<commit_message>
Spawn Randomizer and Enemies
Reworked enemy script as parent class to support more enemy variants. Added random spawning to EvilRectangle.
</commit_message>
<xml_diff>
--- a/BacklogTasks.xlsx
+++ b/BacklogTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnityProjects\DesignAndPublishUnity\CoreRun\CoreRun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232B4A8B-C249-4D2F-91CA-A54EFB4B127B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667EB19D-089F-4E54-A438-2B6837F12F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="277">
   <si>
     <t>Weekly Planning Process</t>
   </si>
@@ -464,18 +464,6 @@
     <t>Background music speeds up with the layers</t>
   </si>
   <si>
-    <t>Define a set interval for layers to increase</t>
-  </si>
-  <si>
-    <t>When a layer increases, change how score is calculated</t>
-  </si>
-  <si>
-    <t>When a layer increases, change the rate at which enemies spawn</t>
-  </si>
-  <si>
-    <t>When a layer increases, change the speed at which the planet rotates</t>
-  </si>
-  <si>
     <t>Refactoring Notes</t>
   </si>
   <si>
@@ -503,57 +491,12 @@
     <t>The Main Menu has a background image</t>
   </si>
   <si>
-    <t>There is a main Menu Screen with a rudimentary background image, music, and settings</t>
-  </si>
-  <si>
-    <t>Detect 'down' input on the player</t>
-  </si>
-  <si>
-    <t>Make the player strafe slower while flattened</t>
-  </si>
-  <si>
-    <t>Add a short cooldown to flattening</t>
-  </si>
-  <si>
     <t>Art</t>
   </si>
   <si>
     <t>Make the Player asset an actual slime</t>
   </si>
   <si>
-    <t>Add an animation when unflattening</t>
-  </si>
-  <si>
-    <t>Add Narrow Dodge function to UI manager</t>
-  </si>
-  <si>
-    <t>Make the function causes a temporary popup to appear near the bottom of the screen saying 'narrow dodge'</t>
-  </si>
-  <si>
-    <t>The popup changes appearance based on the current multiplier</t>
-  </si>
-  <si>
-    <t>Add a sound effects that celebrates when the popup occurs</t>
-  </si>
-  <si>
-    <t>Make the popup appear in random places</t>
-  </si>
-  <si>
-    <t>There are Three different enemies</t>
-  </si>
-  <si>
-    <t>Enemy spawn locations are randomized</t>
-  </si>
-  <si>
-    <t>Define left/right transform limit for spawn location in SpawnManager</t>
-  </si>
-  <si>
-    <t>Define an offset for the rectangle between its' middle and its edge to prevent it from spawning off the road</t>
-  </si>
-  <si>
-    <t>Generate a random left/right movement within boundaries, offset by rectangles limitations</t>
-  </si>
-  <si>
     <t>On the Schedule</t>
   </si>
   <si>
@@ -563,15 +506,6 @@
     <t>Remove scorekeeping responsibilities from GameManager into a new script</t>
   </si>
   <si>
-    <t>Attach Background music to camera and give SoundControl control of it</t>
-  </si>
-  <si>
-    <t>When the game ends, have GameManager tell sound control to stop the music.</t>
-  </si>
-  <si>
-    <t>Make Background music volume adjustable in SoundControl</t>
-  </si>
-  <si>
     <t>SoundControl</t>
   </si>
   <si>
@@ -836,10 +770,106 @@
     <t>The player can press a button to shrink the character</t>
   </si>
   <si>
-    <t>Shrink player in response to down input (ensure collider flattens as well)</t>
-  </si>
-  <si>
     <t>The character animates when shrinking</t>
+  </si>
+  <si>
+    <t>Add some variance to spawn timing</t>
+  </si>
+  <si>
+    <t>Eyes look in the direction of movement</t>
+  </si>
+  <si>
+    <t>Add SFX to shrinking</t>
+  </si>
+  <si>
+    <t>EvilRectangles spawn locations are randomized</t>
+  </si>
+  <si>
+    <t>Implement Big Red</t>
+  </si>
+  <si>
+    <t>Implement Flying Pink</t>
+  </si>
+  <si>
+    <t>There is a main Menu Screen</t>
+  </si>
+  <si>
+    <t>Settings can be accessed from the pause menu</t>
+  </si>
+  <si>
+    <t>Turn the Main Game into a scene</t>
+  </si>
+  <si>
+    <t>Make another scene for the menu</t>
+  </si>
+  <si>
+    <t>Ensure Start button can go to the game scene</t>
+  </si>
+  <si>
+    <t>When the player dies, Let them return to the main menu or quit.</t>
+  </si>
+  <si>
+    <t>Add generic background, settings button, highscore placeholder, and Start/Quit game button</t>
+  </si>
+  <si>
+    <t>Ensure Quit Button Works as intended</t>
+  </si>
+  <si>
+    <t>Remake the character</t>
+  </si>
+  <si>
+    <t>In GameManager, pause the game time when 'Escape' is pressed. Ensure other elements are paused as well.</t>
+  </si>
+  <si>
+    <t>Create a pause Screen that fades the background and shows 'paused' when the game is paused. This should be controlled by UI manager.</t>
+  </si>
+  <si>
+    <t>Reduce music volume by 90% while the game is paused, returning to prior values afterward.</t>
+  </si>
+  <si>
+    <t>The pause menu should have a button to return to main menu.</t>
+  </si>
+  <si>
+    <t>Choose a particle affect to show when the player moves. Load into game, add to list, then make it a child of object the graphic is attached to (not the character!)</t>
+  </si>
+  <si>
+    <t>If the character moves left or right and the opposing horizontal axis is maxed, let it should trigger the particle in that direction.</t>
+  </si>
+  <si>
+    <t>The character should look in the direction their moving</t>
+  </si>
+  <si>
+    <t>The particle size should be based on the character's current size, but not change if the char acter resizes afterwards.</t>
+  </si>
+  <si>
+    <t>Add Big Red sleep mode</t>
+  </si>
+  <si>
+    <t>Make him spawn on either the left or right side.</t>
+  </si>
+  <si>
+    <t>Make him run at the player directly</t>
+  </si>
+  <si>
+    <t>Make him run in zigzags, randomly chosen whether he does zig zags or runs straight</t>
+  </si>
+  <si>
+    <t>Bring Big Red(Teeth Mode) into the scene, give him his own child script. Set his offset so that he fits when facing the player on the left and right sides of the road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have her move between 6 positions in a 2x3 grid. </t>
+  </si>
+  <si>
+    <t>Bring Flying pink into the scene, with her own child script. Have her spawn in the center, offset above the ground above the player collider.</t>
+  </si>
+  <si>
+    <t>Have her move her eyes in the direction she's moving</t>
+  </si>
+  <si>
+    <t>Evil Rectangle should occasionally fall over</t>
+  </si>
+  <si>
+    <t>Have her eyes move in two separate directions, with one of the directions being the place she will move</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1113,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1153,6 +1183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1292,7 +1328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1567,30 +1603,15 @@
     <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1661,6 +1682,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1713,6 +1740,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2047,316 +2080,316 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="126"/>
-      <c r="B1" s="128" t="s">
+      <c r="A1" s="123"/>
+      <c r="B1" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="127"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
+      <c r="A2" s="124"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="127"/>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
+      <c r="A3" s="124"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="127"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="127"/>
+      <c r="A4" s="124"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
     </row>
     <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="127"/>
-      <c r="B5" s="129" t="s">
+      <c r="A5" s="124"/>
+      <c r="B5" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="127"/>
-      <c r="D5" s="127"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
     </row>
     <row r="6" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="127"/>
+      <c r="A6" s="124"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="127"/>
+      <c r="D6" s="124"/>
     </row>
     <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="127"/>
-      <c r="B7" s="129" t="s">
+      <c r="A7" s="124"/>
+      <c r="B7" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="127"/>
-      <c r="D7" s="127"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
     </row>
     <row r="8" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="127"/>
+      <c r="A8" s="124"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="127"/>
+      <c r="D8" s="124"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="127"/>
-      <c r="B9" s="129" t="s">
+      <c r="A9" s="124"/>
+      <c r="B9" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="127"/>
-      <c r="D9" s="127"/>
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
     </row>
     <row r="10" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="127"/>
+      <c r="A10" s="124"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="127"/>
+      <c r="D10" s="124"/>
     </row>
     <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="127"/>
-      <c r="B11" s="129" t="s">
+      <c r="A11" s="124"/>
+      <c r="B11" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="127"/>
-      <c r="D11" s="127"/>
+      <c r="C11" s="124"/>
+      <c r="D11" s="124"/>
     </row>
     <row r="12" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="127"/>
+      <c r="A12" s="124"/>
       <c r="B12" s="5"/>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="127"/>
+      <c r="D12" s="124"/>
     </row>
     <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="127"/>
-      <c r="B13" s="129" t="s">
+      <c r="A13" s="124"/>
+      <c r="B13" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="127"/>
-      <c r="D13" s="127"/>
+      <c r="C13" s="124"/>
+      <c r="D13" s="124"/>
     </row>
     <row r="14" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="127"/>
+      <c r="A14" s="124"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="127"/>
+      <c r="D14" s="124"/>
     </row>
     <row r="15" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="127"/>
-      <c r="B15" s="129" t="s">
+      <c r="A15" s="124"/>
+      <c r="B15" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="127"/>
-      <c r="D15" s="127"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
     </row>
     <row r="16" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="127"/>
+      <c r="A16" s="124"/>
       <c r="B16" s="7"/>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="127"/>
+      <c r="D16" s="124"/>
     </row>
     <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="127"/>
-      <c r="B17" s="126"/>
-      <c r="C17" s="127"/>
-      <c r="D17" s="127"/>
+      <c r="A17" s="124"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="124"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="127"/>
-      <c r="B18" s="127"/>
-      <c r="C18" s="127"/>
-      <c r="D18" s="127"/>
+      <c r="A18" s="124"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="124"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="127"/>
-      <c r="B19" s="127"/>
-      <c r="C19" s="127"/>
-      <c r="D19" s="127"/>
+      <c r="A19" s="124"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="124"/>
+      <c r="D19" s="124"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="127"/>
-      <c r="B20" s="127"/>
-      <c r="C20" s="127"/>
-      <c r="D20" s="127"/>
+      <c r="A20" s="124"/>
+      <c r="B20" s="124"/>
+      <c r="C20" s="124"/>
+      <c r="D20" s="124"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="127"/>
-      <c r="B21" s="127"/>
-      <c r="C21" s="127"/>
-      <c r="D21" s="127"/>
+      <c r="A21" s="124"/>
+      <c r="B21" s="124"/>
+      <c r="C21" s="124"/>
+      <c r="D21" s="124"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="127"/>
-      <c r="B22" s="127"/>
-      <c r="C22" s="127"/>
-      <c r="D22" s="127"/>
+      <c r="A22" s="124"/>
+      <c r="B22" s="124"/>
+      <c r="C22" s="124"/>
+      <c r="D22" s="124"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="127"/>
-      <c r="B23" s="127"/>
-      <c r="C23" s="127"/>
-      <c r="D23" s="127"/>
+      <c r="A23" s="124"/>
+      <c r="B23" s="124"/>
+      <c r="C23" s="124"/>
+      <c r="D23" s="124"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="127"/>
-      <c r="B24" s="127"/>
-      <c r="C24" s="127"/>
-      <c r="D24" s="127"/>
+      <c r="A24" s="124"/>
+      <c r="B24" s="124"/>
+      <c r="C24" s="124"/>
+      <c r="D24" s="124"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="127"/>
-      <c r="B25" s="127"/>
-      <c r="C25" s="127"/>
-      <c r="D25" s="127"/>
+      <c r="A25" s="124"/>
+      <c r="B25" s="124"/>
+      <c r="C25" s="124"/>
+      <c r="D25" s="124"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="127"/>
-      <c r="B26" s="127"/>
-      <c r="C26" s="127"/>
-      <c r="D26" s="127"/>
+      <c r="A26" s="124"/>
+      <c r="B26" s="124"/>
+      <c r="C26" s="124"/>
+      <c r="D26" s="124"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="127"/>
-      <c r="B27" s="127"/>
-      <c r="C27" s="127"/>
-      <c r="D27" s="127"/>
+      <c r="A27" s="124"/>
+      <c r="B27" s="124"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="124"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="127"/>
-      <c r="B28" s="127"/>
-      <c r="C28" s="127"/>
-      <c r="D28" s="127"/>
+      <c r="A28" s="124"/>
+      <c r="B28" s="124"/>
+      <c r="C28" s="124"/>
+      <c r="D28" s="124"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="127"/>
-      <c r="B29" s="127"/>
-      <c r="C29" s="127"/>
-      <c r="D29" s="127"/>
+      <c r="A29" s="124"/>
+      <c r="B29" s="124"/>
+      <c r="C29" s="124"/>
+      <c r="D29" s="124"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="127"/>
-      <c r="B30" s="127"/>
-      <c r="C30" s="127"/>
-      <c r="D30" s="127"/>
+      <c r="A30" s="124"/>
+      <c r="B30" s="124"/>
+      <c r="C30" s="124"/>
+      <c r="D30" s="124"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="127"/>
-      <c r="B31" s="127"/>
-      <c r="C31" s="127"/>
-      <c r="D31" s="127"/>
+      <c r="A31" s="124"/>
+      <c r="B31" s="124"/>
+      <c r="C31" s="124"/>
+      <c r="D31" s="124"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="127"/>
-      <c r="B32" s="127"/>
-      <c r="C32" s="127"/>
-      <c r="D32" s="127"/>
+      <c r="A32" s="124"/>
+      <c r="B32" s="124"/>
+      <c r="C32" s="124"/>
+      <c r="D32" s="124"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="127"/>
-      <c r="B33" s="127"/>
-      <c r="C33" s="127"/>
-      <c r="D33" s="127"/>
+      <c r="A33" s="124"/>
+      <c r="B33" s="124"/>
+      <c r="C33" s="124"/>
+      <c r="D33" s="124"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="127"/>
-      <c r="B34" s="127"/>
-      <c r="C34" s="127"/>
-      <c r="D34" s="127"/>
+      <c r="A34" s="124"/>
+      <c r="B34" s="124"/>
+      <c r="C34" s="124"/>
+      <c r="D34" s="124"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="127"/>
-      <c r="B35" s="127"/>
-      <c r="C35" s="127"/>
-      <c r="D35" s="127"/>
+      <c r="A35" s="124"/>
+      <c r="B35" s="124"/>
+      <c r="C35" s="124"/>
+      <c r="D35" s="124"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="127"/>
-      <c r="B36" s="127"/>
-      <c r="C36" s="127"/>
-      <c r="D36" s="127"/>
+      <c r="A36" s="124"/>
+      <c r="B36" s="124"/>
+      <c r="C36" s="124"/>
+      <c r="D36" s="124"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="127"/>
-      <c r="B37" s="127"/>
-      <c r="C37" s="127"/>
-      <c r="D37" s="127"/>
+      <c r="A37" s="124"/>
+      <c r="B37" s="124"/>
+      <c r="C37" s="124"/>
+      <c r="D37" s="124"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="127"/>
-      <c r="B38" s="127"/>
-      <c r="C38" s="127"/>
-      <c r="D38" s="127"/>
+      <c r="A38" s="124"/>
+      <c r="B38" s="124"/>
+      <c r="C38" s="124"/>
+      <c r="D38" s="124"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="127"/>
-      <c r="B39" s="127"/>
-      <c r="C39" s="127"/>
-      <c r="D39" s="127"/>
+      <c r="A39" s="124"/>
+      <c r="B39" s="124"/>
+      <c r="C39" s="124"/>
+      <c r="D39" s="124"/>
     </row>
     <row r="40" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="127"/>
+      <c r="A40" s="124"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="127"/>
+      <c r="D40" s="124"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="127"/>
+      <c r="A41" s="124"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="127"/>
+      <c r="D41" s="124"/>
     </row>
     <row r="42" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="127"/>
+      <c r="A42" s="124"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="127"/>
+      <c r="A43" s="124"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="127"/>
+      <c r="A44" s="124"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="127"/>
+      <c r="A45" s="124"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="127"/>
+      <c r="A46" s="124"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="127"/>
+      <c r="A47" s="124"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="127"/>
+      <c r="A48" s="124"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="127"/>
+      <c r="A49" s="124"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
@@ -2422,15 +2455,15 @@
     </row>
     <row r="2" spans="1:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
       <c r="I2" s="8"/>
       <c r="J2" s="10"/>
       <c r="K2" s="9"/>
@@ -2473,14 +2506,14 @@
       <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="134" t="s">
+      <c r="C4" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="135"/>
-      <c r="E4" s="134" t="s">
+      <c r="D4" s="132"/>
+      <c r="E4" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="136"/>
+      <c r="F4" s="133"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2499,14 +2532,14 @@
     <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
-      <c r="C5" s="137" t="s">
+      <c r="C5" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="127"/>
-      <c r="E5" s="137" t="s">
+      <c r="D5" s="124"/>
+      <c r="E5" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="138"/>
+      <c r="F5" s="135"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2525,14 +2558,14 @@
     <row r="6" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
-      <c r="C6" s="137" t="s">
+      <c r="C6" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="127"/>
-      <c r="E6" s="137" t="s">
+      <c r="D6" s="124"/>
+      <c r="E6" s="134" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="138"/>
+      <c r="F6" s="135"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -2551,14 +2584,14 @@
     <row r="7" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="130" t="s">
+      <c r="C7" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="131"/>
-      <c r="E7" s="130" t="s">
+      <c r="D7" s="128"/>
+      <c r="E7" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="132"/>
+      <c r="F7" s="129"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -4972,11 +5005,11 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="139" t="s">
+      <c r="D4" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -5322,104 +5355,104 @@
       <c r="Y14" s="1"/>
     </row>
     <row r="15" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="126"/>
-      <c r="B15" s="127"/>
-      <c r="C15" s="127"/>
-      <c r="D15" s="127"/>
-      <c r="E15" s="127"/>
-      <c r="F15" s="127"/>
-      <c r="G15" s="127"/>
-      <c r="H15" s="127"/>
-      <c r="I15" s="127"/>
-      <c r="J15" s="127"/>
-      <c r="K15" s="127"/>
-      <c r="L15" s="127"/>
-      <c r="M15" s="127"/>
-      <c r="N15" s="127"/>
-      <c r="O15" s="127"/>
-      <c r="P15" s="127"/>
-      <c r="Q15" s="127"/>
-      <c r="R15" s="127"/>
-      <c r="S15" s="127"/>
-      <c r="T15" s="127"/>
-      <c r="U15" s="127"/>
-      <c r="V15" s="127"/>
-      <c r="W15" s="127"/>
-      <c r="X15" s="127"/>
-      <c r="Y15" s="127"/>
+      <c r="A15" s="123"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="124"/>
+      <c r="O15" s="124"/>
+      <c r="P15" s="124"/>
+      <c r="Q15" s="124"/>
+      <c r="R15" s="124"/>
+      <c r="S15" s="124"/>
+      <c r="T15" s="124"/>
+      <c r="U15" s="124"/>
+      <c r="V15" s="124"/>
+      <c r="W15" s="124"/>
+      <c r="X15" s="124"/>
+      <c r="Y15" s="124"/>
     </row>
     <row r="16" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="127"/>
-      <c r="B16" s="127"/>
-      <c r="C16" s="127"/>
-      <c r="D16" s="127"/>
-      <c r="E16" s="127"/>
-      <c r="F16" s="127"/>
-      <c r="G16" s="127"/>
-      <c r="H16" s="127"/>
-      <c r="I16" s="127"/>
-      <c r="J16" s="127"/>
-      <c r="K16" s="127"/>
-      <c r="L16" s="127"/>
-      <c r="M16" s="127"/>
-      <c r="N16" s="127"/>
-      <c r="O16" s="127"/>
-      <c r="P16" s="127"/>
-      <c r="Q16" s="127"/>
-      <c r="R16" s="127"/>
-      <c r="S16" s="127"/>
-      <c r="T16" s="127"/>
-      <c r="U16" s="127"/>
-      <c r="V16" s="127"/>
-      <c r="W16" s="127"/>
-      <c r="X16" s="127"/>
-      <c r="Y16" s="127"/>
+      <c r="A16" s="124"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="124"/>
+      <c r="D16" s="124"/>
+      <c r="E16" s="124"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
+      <c r="H16" s="124"/>
+      <c r="I16" s="124"/>
+      <c r="J16" s="124"/>
+      <c r="K16" s="124"/>
+      <c r="L16" s="124"/>
+      <c r="M16" s="124"/>
+      <c r="N16" s="124"/>
+      <c r="O16" s="124"/>
+      <c r="P16" s="124"/>
+      <c r="Q16" s="124"/>
+      <c r="R16" s="124"/>
+      <c r="S16" s="124"/>
+      <c r="T16" s="124"/>
+      <c r="U16" s="124"/>
+      <c r="V16" s="124"/>
+      <c r="W16" s="124"/>
+      <c r="X16" s="124"/>
+      <c r="Y16" s="124"/>
     </row>
     <row r="17" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="127"/>
-      <c r="B17" s="127"/>
-      <c r="C17" s="127"/>
-      <c r="D17" s="127"/>
-      <c r="E17" s="127"/>
-      <c r="F17" s="127"/>
-      <c r="G17" s="127"/>
-      <c r="H17" s="127"/>
-      <c r="I17" s="127"/>
-      <c r="J17" s="127"/>
-      <c r="K17" s="127"/>
-      <c r="L17" s="127"/>
-      <c r="M17" s="127"/>
-      <c r="N17" s="127"/>
-      <c r="O17" s="127"/>
-      <c r="P17" s="127"/>
-      <c r="Q17" s="127"/>
-      <c r="R17" s="127"/>
-      <c r="S17" s="127"/>
-      <c r="T17" s="127"/>
-      <c r="U17" s="127"/>
-      <c r="V17" s="127"/>
-      <c r="W17" s="127"/>
-      <c r="X17" s="127"/>
-      <c r="Y17" s="127"/>
+      <c r="A17" s="124"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="124"/>
+      <c r="E17" s="124"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="124"/>
+      <c r="H17" s="124"/>
+      <c r="I17" s="124"/>
+      <c r="J17" s="124"/>
+      <c r="K17" s="124"/>
+      <c r="L17" s="124"/>
+      <c r="M17" s="124"/>
+      <c r="N17" s="124"/>
+      <c r="O17" s="124"/>
+      <c r="P17" s="124"/>
+      <c r="Q17" s="124"/>
+      <c r="R17" s="124"/>
+      <c r="S17" s="124"/>
+      <c r="T17" s="124"/>
+      <c r="U17" s="124"/>
+      <c r="V17" s="124"/>
+      <c r="W17" s="124"/>
+      <c r="X17" s="124"/>
+      <c r="Y17" s="124"/>
     </row>
     <row r="18" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="29"/>
-      <c r="C18" s="140" t="s">
+      <c r="C18" s="137" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="127"/>
-      <c r="E18" s="127"/>
-      <c r="F18" s="127"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="124"/>
       <c r="G18" s="29"/>
       <c r="H18" s="1"/>
       <c r="I18" s="29"/>
-      <c r="J18" s="140" t="s">
+      <c r="J18" s="137" t="s">
         <v>55</v>
       </c>
-      <c r="K18" s="127"/>
-      <c r="L18" s="127"/>
-      <c r="M18" s="127"/>
+      <c r="K18" s="124"/>
+      <c r="L18" s="124"/>
+      <c r="M18" s="124"/>
       <c r="N18" s="29"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -6089,15 +6122,15 @@
       <c r="A39" s="1"/>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
-      <c r="D39" s="141"/>
-      <c r="E39" s="127"/>
+      <c r="D39" s="138"/>
+      <c r="E39" s="124"/>
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
       <c r="H39" s="1"/>
       <c r="I39" s="29"/>
       <c r="J39" s="29"/>
-      <c r="K39" s="141"/>
-      <c r="L39" s="127"/>
+      <c r="K39" s="138"/>
+      <c r="L39" s="124"/>
       <c r="M39" s="29"/>
       <c r="N39" s="29"/>
       <c r="O39" s="12"/>
@@ -7669,10 +7702,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T112"/>
+  <dimension ref="A1:T114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7691,14 +7724,14 @@
       <c r="B1" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="142" t="s">
+      <c r="C1" s="139" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="127"/>
-      <c r="E1" s="142" t="s">
+      <c r="D1" s="124"/>
+      <c r="E1" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="138"/>
+      <c r="F1" s="135"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -7717,14 +7750,14 @@
     <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
-      <c r="C2" s="137" t="s">
+      <c r="C2" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="137" t="s">
+      <c r="D2" s="124"/>
+      <c r="E2" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="138"/>
+      <c r="F2" s="135"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -7743,14 +7776,14 @@
     <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
-      <c r="C3" s="137" t="s">
+      <c r="C3" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="127"/>
-      <c r="E3" s="137" t="s">
+      <c r="D3" s="124"/>
+      <c r="E3" s="134" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="138"/>
+      <c r="F3" s="135"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -7769,14 +7802,14 @@
     <row r="4" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
-      <c r="C4" s="130" t="s">
+      <c r="C4" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="131"/>
-      <c r="E4" s="130" t="s">
+      <c r="D4" s="128"/>
+      <c r="E4" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="132"/>
+      <c r="F4" s="129"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -7802,7 +7835,7 @@
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="105"/>
+      <c r="H5" s="100"/>
       <c r="I5" s="64"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -7832,7 +7865,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="65"/>
       <c r="I6" s="64" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -7904,45 +7937,45 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" s="122" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="42"/>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="121" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" s="121">
+        <v>2</v>
+      </c>
+      <c r="D9" s="121"/>
+      <c r="E9" s="121">
+        <v>2</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="121"/>
+      <c r="R9" s="121"/>
+      <c r="S9" s="121"/>
+      <c r="T9" s="121"/>
+    </row>
+    <row r="10" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="42"/>
+      <c r="B10" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="47">
-        <v>3</v>
-      </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47">
+      <c r="C10" s="47">
         <v>2</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="47"/>
-    </row>
-    <row r="10" spans="1:20" s="46" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
-      <c r="B10" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="47">
-        <v>3</v>
       </c>
       <c r="D10" s="47"/>
       <c r="E10" s="47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="47"/>
@@ -7960,13 +7993,13 @@
       <c r="S10" s="47"/>
       <c r="T10" s="47"/>
     </row>
-    <row r="11" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="46" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="42"/>
-      <c r="B11" s="62" t="s">
-        <v>98</v>
+      <c r="B11" s="47" t="s">
+        <v>80</v>
       </c>
       <c r="C11" s="47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="47"/>
       <c r="E11" s="47">
@@ -7988,69 +8021,69 @@
       <c r="S11" s="47"/>
       <c r="T11" s="47"/>
     </row>
-    <row r="12" spans="1:20" s="48" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="42"/>
       <c r="B12" s="62" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" s="49">
+        <v>98</v>
+      </c>
+      <c r="C12" s="47">
         <v>2</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49">
-        <v>3</v>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47">
+        <v>1</v>
       </c>
       <c r="F12" s="18"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="49"/>
-      <c r="S12" s="49"/>
-      <c r="T12" s="49"/>
-    </row>
-    <row r="13" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+    </row>
+    <row r="13" spans="1:20" s="48" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="42"/>
       <c r="B13" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="47">
+        <v>99</v>
+      </c>
+      <c r="C13" s="49">
         <v>2</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47">
-        <v>2</v>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49">
+        <v>3</v>
       </c>
       <c r="F13" s="18"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="47"/>
-      <c r="Q13" s="47"/>
-      <c r="R13" s="47"/>
-      <c r="S13" s="47"/>
-      <c r="T13" s="47"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
     </row>
     <row r="14" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="42"/>
-      <c r="B14" s="47" t="s">
-        <v>85</v>
+      <c r="B14" s="62" t="s">
+        <v>86</v>
       </c>
       <c r="C14" s="47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="47"/>
       <c r="E14" s="47">
@@ -8072,94 +8105,98 @@
       <c r="S14" s="47"/>
       <c r="T14" s="47"/>
     </row>
-    <row r="15" spans="1:20" s="123" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="42"/>
-      <c r="B15" s="122" t="s">
-        <v>266</v>
-      </c>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
-      <c r="E15" s="122"/>
+      <c r="B15" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="47">
+        <v>3</v>
+      </c>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47">
+        <v>2</v>
+      </c>
       <c r="F15" s="18"/>
-      <c r="G15" s="122"/>
-      <c r="H15" s="122"/>
-      <c r="I15" s="122"/>
-      <c r="J15" s="122"/>
-      <c r="K15" s="122"/>
-      <c r="L15" s="122"/>
-      <c r="M15" s="122"/>
-      <c r="N15" s="122"/>
-      <c r="O15" s="122"/>
-      <c r="P15" s="122"/>
-      <c r="Q15" s="122"/>
-      <c r="R15" s="122"/>
-      <c r="S15" s="122"/>
-      <c r="T15" s="122"/>
-    </row>
-    <row r="16" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+    </row>
+    <row r="16" spans="1:20" s="118" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="42"/>
-      <c r="B16" s="62" t="s">
-        <v>264</v>
-      </c>
-      <c r="C16" s="47">
+      <c r="B16" s="117" t="s">
+        <v>243</v>
+      </c>
+      <c r="C16" s="117">
+        <v>3</v>
+      </c>
+      <c r="D16" s="117"/>
+      <c r="E16" s="117">
         <v>2</v>
       </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47">
+      <c r="F16" s="18"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="117"/>
+      <c r="I16" s="117"/>
+      <c r="J16" s="117"/>
+      <c r="K16" s="117"/>
+      <c r="L16" s="117"/>
+      <c r="M16" s="117"/>
+      <c r="N16" s="117"/>
+      <c r="O16" s="117"/>
+      <c r="P16" s="117"/>
+      <c r="Q16" s="117"/>
+      <c r="R16" s="117"/>
+      <c r="S16" s="117"/>
+      <c r="T16" s="117"/>
+    </row>
+    <row r="17" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="42"/>
+      <c r="B17" s="62" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" s="47">
+        <v>2</v>
+      </c>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47">
         <v>3</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
-      <c r="Q16" s="47"/>
-      <c r="R16" s="47"/>
-      <c r="S16" s="47"/>
-      <c r="T16" s="47"/>
-    </row>
-    <row r="17" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="43" t="s">
+      <c r="F17" s="18"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
+    </row>
+    <row r="18" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="41"/>
-      <c r="B18" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1">
-        <v>2</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="18"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -8176,13 +8213,13 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="41"/>
-      <c r="B19" s="62" t="s">
-        <v>81</v>
+      <c r="B19" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1">
@@ -8207,14 +8244,14 @@
     <row r="20" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="41"/>
       <c r="B20" s="62" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="1"/>
@@ -8232,182 +8269,182 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" s="46" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
-      <c r="B21" s="86" t="s">
-        <v>167</v>
-      </c>
-      <c r="C21" s="47">
+    <row r="21" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="41"/>
+      <c r="B21" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="42"/>
+      <c r="B22" s="62" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="47">
         <v>2</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47">
+      <c r="D22" s="47"/>
+      <c r="E22" s="47">
         <v>2</v>
       </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
-    </row>
-    <row r="22" spans="1:20" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
-      <c r="B22" s="49" t="s">
-        <v>166</v>
-      </c>
-      <c r="C22" s="49">
+      <c r="F22" s="18"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="47"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
+    </row>
+    <row r="23" spans="1:20" s="122" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="42"/>
+      <c r="B23" s="86" t="s">
+        <v>248</v>
+      </c>
+      <c r="C23" s="121">
         <v>2</v>
       </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49">
+      <c r="D23" s="121"/>
+      <c r="E23" s="121">
+        <v>2</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="121"/>
+      <c r="H23" s="121"/>
+      <c r="I23" s="121"/>
+      <c r="J23" s="121"/>
+      <c r="K23" s="121"/>
+      <c r="L23" s="121"/>
+      <c r="M23" s="121"/>
+      <c r="N23" s="121"/>
+      <c r="O23" s="121"/>
+      <c r="P23" s="121"/>
+      <c r="Q23" s="121"/>
+      <c r="R23" s="121"/>
+      <c r="S23" s="121"/>
+      <c r="T23" s="121"/>
+    </row>
+    <row r="24" spans="1:20" s="48" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="42"/>
+      <c r="B24" s="86" t="s">
+        <v>249</v>
+      </c>
+      <c r="C24" s="49">
+        <v>2</v>
+      </c>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49">
+        <v>2</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+    </row>
+    <row r="25" spans="1:20" s="61" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="42"/>
+      <c r="B25" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="60">
+        <v>1</v>
+      </c>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60">
         <v>3</v>
       </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
-      <c r="Q22" s="49"/>
-      <c r="R22" s="49"/>
-      <c r="S22" s="49"/>
-      <c r="T22" s="49"/>
-    </row>
-    <row r="23" spans="1:20" s="61" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
-      <c r="B23" s="75" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="60">
-        <v>1</v>
-      </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60">
+      <c r="F25" s="18"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="60"/>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="60"/>
+      <c r="S25" s="60"/>
+      <c r="T25" s="60"/>
+    </row>
+    <row r="26" spans="1:20" s="46" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="42"/>
+      <c r="B26" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="47">
         <v>3</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="60"/>
-      <c r="T23" s="60"/>
-    </row>
-    <row r="24" spans="1:20" s="46" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
-      <c r="B24" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="47">
-        <v>3</v>
-      </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47">
+      <c r="D26" s="47"/>
+      <c r="E26" s="47">
         <v>2</v>
       </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47"/>
-      <c r="Q24" s="47"/>
-      <c r="R24" s="47"/>
-      <c r="S24" s="47"/>
-      <c r="T24" s="47"/>
-    </row>
-    <row r="25" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="43" t="s">
+      <c r="F26" s="18"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="47"/>
+    </row>
+    <row r="27" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-    </row>
-    <row r="26" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="41"/>
-      <c r="B26" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="18"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-    </row>
-    <row r="27" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="41"/>
-      <c r="B27" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="1">
-        <v>3</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1">
-        <v>3</v>
-      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="18"/>
       <c r="G27" s="20"/>
       <c r="H27" s="1"/>
@@ -8424,42 +8461,46 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
-      <c r="B28" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="47">
-        <v>2</v>
-      </c>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47">
-        <v>3</v>
+    <row r="28" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="41"/>
+      <c r="B28" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1">
+        <v>1</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="20"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="47"/>
-      <c r="P28" s="47"/>
-      <c r="Q28" s="47"/>
-      <c r="R28" s="47"/>
-      <c r="S28" s="47"/>
-      <c r="T28" s="47"/>
-    </row>
-    <row r="29" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+    </row>
+    <row r="29" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="41"/>
+      <c r="B29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3</v>
+      </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1">
+        <v>3</v>
+      </c>
       <c r="F29" s="18"/>
       <c r="G29" s="20"/>
       <c r="H29" s="1"/>
@@ -8476,46 +8517,42 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="41"/>
-      <c r="B30" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1">
-        <v>1</v>
+    <row r="30" spans="1:20" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="42"/>
+      <c r="B30" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="47">
+        <v>2</v>
+      </c>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47">
+        <v>3</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="20"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-    </row>
-    <row r="31" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-      <c r="B31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="1">
-        <v>3</v>
-      </c>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="47"/>
+      <c r="P30" s="47"/>
+      <c r="Q30" s="47"/>
+      <c r="R30" s="47"/>
+      <c r="S30" s="47"/>
+      <c r="T30" s="47"/>
+    </row>
+    <row r="31" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1">
-        <v>2</v>
-      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="18"/>
       <c r="G31" s="20"/>
       <c r="H31" s="1"/>
@@ -8532,126 +8569,126 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" s="77" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="43"/>
+    <row r="32" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="41"/>
       <c r="B32" s="62" t="s">
-        <v>139</v>
-      </c>
-      <c r="C32" s="76">
-        <v>2</v>
-      </c>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76">
-        <v>2</v>
+        <v>89</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1">
+        <v>1</v>
       </c>
       <c r="F32" s="18"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="76"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="76"/>
-      <c r="K32" s="76"/>
-      <c r="L32" s="76"/>
-      <c r="M32" s="76"/>
-      <c r="N32" s="76"/>
-      <c r="O32" s="76"/>
-      <c r="P32" s="76"/>
-      <c r="Q32" s="76"/>
-      <c r="R32" s="76"/>
-      <c r="S32" s="76"/>
-      <c r="T32" s="76"/>
-    </row>
-    <row r="33" spans="1:20" s="52" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
-      <c r="B33" s="51" t="s">
-        <v>138</v>
-      </c>
-      <c r="C33" s="51">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+    </row>
+    <row r="33" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="17"/>
+      <c r="B33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="1">
         <v>3</v>
       </c>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51">
-        <v>3</v>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1">
+        <v>2</v>
       </c>
       <c r="F33" s="18"/>
       <c r="G33" s="20"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="51"/>
-      <c r="P33" s="51"/>
-      <c r="Q33" s="51"/>
-      <c r="R33" s="51"/>
-      <c r="S33" s="51"/>
-      <c r="T33" s="51"/>
-    </row>
-    <row r="34" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+    </row>
+    <row r="34" spans="1:20" s="77" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="43"/>
+      <c r="B34" s="62" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="76">
+        <v>2</v>
+      </c>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76">
+        <v>2</v>
+      </c>
       <c r="F34" s="18"/>
       <c r="G34" s="20"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-    </row>
-    <row r="35" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="41"/>
-      <c r="B35" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" s="1">
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="76"/>
+      <c r="P34" s="76"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="76"/>
+      <c r="S34" s="76"/>
+      <c r="T34" s="76"/>
+    </row>
+    <row r="35" spans="1:20" s="52" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="42"/>
+      <c r="B35" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="51">
         <v>3</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1">
-        <v>1</v>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51">
+        <v>3</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="20"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-    </row>
-    <row r="36" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="1">
-        <v>3</v>
-      </c>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="51"/>
+      <c r="O35" s="51"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="51"/>
+      <c r="R35" s="51"/>
+      <c r="S35" s="51"/>
+      <c r="T35" s="51"/>
+    </row>
+    <row r="36" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1">
-        <v>1</v>
-      </c>
+      <c r="E36" s="1"/>
       <c r="F36" s="18"/>
       <c r="G36" s="20"/>
       <c r="H36" s="1"/>
@@ -8668,73 +8705,73 @@
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="44"/>
-      <c r="B37" s="62" t="s">
-        <v>94</v>
+    <row r="37" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="41"/>
+      <c r="B37" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C37" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1">
         <v>1</v>
       </c>
-      <c r="F37" s="22"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="21"/>
-      <c r="O37" s="21"/>
-      <c r="P37" s="21"/>
-      <c r="Q37" s="21"/>
-      <c r="R37" s="21"/>
-      <c r="S37" s="21"/>
-      <c r="T37" s="21"/>
-    </row>
-    <row r="38" spans="1:20" s="79" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="44"/>
-      <c r="B38" s="103" t="s">
-        <v>181</v>
-      </c>
-      <c r="C38" s="78">
+      <c r="F37" s="18"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+    </row>
+    <row r="38" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="1">
         <v>3</v>
       </c>
-      <c r="D38" s="78"/>
-      <c r="E38" s="78">
-        <v>3</v>
-      </c>
-      <c r="F38" s="22"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="21"/>
-      <c r="O38" s="21"/>
-      <c r="P38" s="21"/>
-      <c r="Q38" s="21"/>
-      <c r="R38" s="21"/>
-      <c r="S38" s="21"/>
-      <c r="T38" s="21"/>
-    </row>
-    <row r="39" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="18"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+    </row>
+    <row r="39" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="44"/>
-      <c r="B39" s="1" t="s">
-        <v>140</v>
+      <c r="B39" s="62" t="s">
+        <v>94</v>
       </c>
       <c r="C39" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="23"/>
@@ -8752,70 +8789,70 @@
       <c r="S39" s="21"/>
       <c r="T39" s="21"/>
     </row>
-    <row r="40" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-    </row>
-    <row r="41" spans="1:20" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="41"/>
+    <row r="40" spans="1:20" s="79" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="44"/>
+      <c r="B40" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="C40" s="78">
+        <v>3</v>
+      </c>
+      <c r="D40" s="78"/>
+      <c r="E40" s="78">
+        <v>3</v>
+      </c>
+      <c r="F40" s="22"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="21"/>
+    </row>
+    <row r="41" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="44"/>
       <c r="B41" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="C41" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1">
-        <v>3</v>
-      </c>
-      <c r="F41" s="18"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F41" s="22"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
     </row>
     <row r="42" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C42" s="1">
-        <v>3</v>
-      </c>
+      <c r="A42" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="1">
-        <v>3</v>
-      </c>
+      <c r="E42" s="1"/>
       <c r="F42" s="18"/>
       <c r="G42" s="20"/>
       <c r="H42" s="1"/>
@@ -8833,16 +8870,16 @@
       <c r="T42" s="1"/>
     </row>
     <row r="43" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1" t="s">
-        <v>153</v>
+      <c r="A43" s="41"/>
+      <c r="B43" s="86" t="s">
+        <v>250</v>
       </c>
       <c r="C43" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F43" s="18"/>
       <c r="G43" s="20"/>
@@ -8863,10 +8900,10 @@
     <row r="44" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="C44" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1">
@@ -8890,10 +8927,16 @@
     </row>
     <row r="45" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3</v>
+      </c>
       <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
+      <c r="E45" s="1">
+        <v>2</v>
+      </c>
       <c r="F45" s="18"/>
       <c r="G45" s="20"/>
       <c r="H45" s="1"/>
@@ -8912,10 +8955,16 @@
     </row>
     <row r="46" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="B46" s="86" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="E46" s="1">
+        <v>3</v>
+      </c>
       <c r="F46" s="18"/>
       <c r="G46" s="20"/>
       <c r="H46" s="1"/>
@@ -8932,9 +8981,11 @@
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
     </row>
-    <row r="47" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -10383,6 +10434,50 @@
       <c r="R112" s="1"/>
       <c r="S112" s="1"/>
       <c r="T112" s="1"/>
+    </row>
+    <row r="113" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="18"/>
+      <c r="G113" s="20"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1"/>
+      <c r="P113" s="1"/>
+      <c r="Q113" s="1"/>
+      <c r="R113" s="1"/>
+      <c r="S113" s="1"/>
+      <c r="T113" s="1"/>
+    </row>
+    <row r="114" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="20"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+      <c r="O114" s="1"/>
+      <c r="P114" s="1"/>
+      <c r="Q114" s="1"/>
+      <c r="R114" s="1"/>
+      <c r="S114" s="1"/>
+      <c r="T114" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -10407,8 +10502,8 @@
   </sheetPr>
   <dimension ref="A1:Y96"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10514,11 +10609,11 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="139" t="s">
+      <c r="D4" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -10864,104 +10959,104 @@
       <c r="Y14" s="1"/>
     </row>
     <row r="15" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="126"/>
-      <c r="B15" s="127"/>
-      <c r="C15" s="127"/>
-      <c r="D15" s="127"/>
-      <c r="E15" s="127"/>
-      <c r="F15" s="127"/>
-      <c r="G15" s="127"/>
-      <c r="H15" s="127"/>
-      <c r="I15" s="127"/>
-      <c r="J15" s="127"/>
-      <c r="K15" s="127"/>
-      <c r="L15" s="127"/>
-      <c r="M15" s="127"/>
-      <c r="N15" s="127"/>
-      <c r="O15" s="127"/>
-      <c r="P15" s="127"/>
-      <c r="Q15" s="127"/>
-      <c r="R15" s="127"/>
-      <c r="S15" s="127"/>
-      <c r="T15" s="127"/>
-      <c r="U15" s="127"/>
-      <c r="V15" s="127"/>
-      <c r="W15" s="127"/>
-      <c r="X15" s="127"/>
-      <c r="Y15" s="127"/>
+      <c r="A15" s="123"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="124"/>
+      <c r="O15" s="124"/>
+      <c r="P15" s="124"/>
+      <c r="Q15" s="124"/>
+      <c r="R15" s="124"/>
+      <c r="S15" s="124"/>
+      <c r="T15" s="124"/>
+      <c r="U15" s="124"/>
+      <c r="V15" s="124"/>
+      <c r="W15" s="124"/>
+      <c r="X15" s="124"/>
+      <c r="Y15" s="124"/>
     </row>
     <row r="16" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="127"/>
-      <c r="B16" s="127"/>
-      <c r="C16" s="127"/>
-      <c r="D16" s="127"/>
-      <c r="E16" s="127"/>
-      <c r="F16" s="127"/>
-      <c r="G16" s="127"/>
-      <c r="H16" s="127"/>
-      <c r="I16" s="127"/>
-      <c r="J16" s="127"/>
-      <c r="K16" s="127"/>
-      <c r="L16" s="127"/>
-      <c r="M16" s="127"/>
-      <c r="N16" s="127"/>
-      <c r="O16" s="127"/>
-      <c r="P16" s="127"/>
-      <c r="Q16" s="127"/>
-      <c r="R16" s="127"/>
-      <c r="S16" s="127"/>
-      <c r="T16" s="127"/>
-      <c r="U16" s="127"/>
-      <c r="V16" s="127"/>
-      <c r="W16" s="127"/>
-      <c r="X16" s="127"/>
-      <c r="Y16" s="127"/>
+      <c r="A16" s="124"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="124"/>
+      <c r="D16" s="124"/>
+      <c r="E16" s="124"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
+      <c r="H16" s="124"/>
+      <c r="I16" s="124"/>
+      <c r="J16" s="124"/>
+      <c r="K16" s="124"/>
+      <c r="L16" s="124"/>
+      <c r="M16" s="124"/>
+      <c r="N16" s="124"/>
+      <c r="O16" s="124"/>
+      <c r="P16" s="124"/>
+      <c r="Q16" s="124"/>
+      <c r="R16" s="124"/>
+      <c r="S16" s="124"/>
+      <c r="T16" s="124"/>
+      <c r="U16" s="124"/>
+      <c r="V16" s="124"/>
+      <c r="W16" s="124"/>
+      <c r="X16" s="124"/>
+      <c r="Y16" s="124"/>
     </row>
     <row r="17" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="127"/>
-      <c r="B17" s="127"/>
-      <c r="C17" s="127"/>
-      <c r="D17" s="127"/>
-      <c r="E17" s="127"/>
-      <c r="F17" s="127"/>
-      <c r="G17" s="127"/>
-      <c r="H17" s="127"/>
-      <c r="I17" s="127"/>
-      <c r="J17" s="127"/>
-      <c r="K17" s="127"/>
-      <c r="L17" s="127"/>
-      <c r="M17" s="127"/>
-      <c r="N17" s="127"/>
-      <c r="O17" s="127"/>
-      <c r="P17" s="127"/>
-      <c r="Q17" s="127"/>
-      <c r="R17" s="127"/>
-      <c r="S17" s="127"/>
-      <c r="T17" s="127"/>
-      <c r="U17" s="127"/>
-      <c r="V17" s="127"/>
-      <c r="W17" s="127"/>
-      <c r="X17" s="127"/>
-      <c r="Y17" s="127"/>
+      <c r="A17" s="124"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="124"/>
+      <c r="E17" s="124"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="124"/>
+      <c r="H17" s="124"/>
+      <c r="I17" s="124"/>
+      <c r="J17" s="124"/>
+      <c r="K17" s="124"/>
+      <c r="L17" s="124"/>
+      <c r="M17" s="124"/>
+      <c r="N17" s="124"/>
+      <c r="O17" s="124"/>
+      <c r="P17" s="124"/>
+      <c r="Q17" s="124"/>
+      <c r="R17" s="124"/>
+      <c r="S17" s="124"/>
+      <c r="T17" s="124"/>
+      <c r="U17" s="124"/>
+      <c r="V17" s="124"/>
+      <c r="W17" s="124"/>
+      <c r="X17" s="124"/>
+      <c r="Y17" s="124"/>
     </row>
     <row r="18" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="53"/>
       <c r="B18" s="55"/>
-      <c r="C18" s="145" t="s">
+      <c r="C18" s="142" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="144"/>
-      <c r="E18" s="144"/>
-      <c r="F18" s="144"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
       <c r="G18" s="55"/>
       <c r="H18" s="53"/>
       <c r="I18" s="55"/>
-      <c r="J18" s="145" t="s">
+      <c r="J18" s="142" t="s">
         <v>97</v>
       </c>
-      <c r="K18" s="144"/>
-      <c r="L18" s="144"/>
-      <c r="M18" s="144"/>
+      <c r="K18" s="141"/>
+      <c r="L18" s="141"/>
+      <c r="M18" s="141"/>
       <c r="N18" s="29"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -11023,29 +11118,29 @@
     <row r="20" spans="1:25" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="53"/>
       <c r="B20" s="55"/>
-      <c r="C20" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="D20" s="100">
+      <c r="C20" s="54" t="s">
+        <v>250</v>
+      </c>
+      <c r="D20" s="81">
         <v>2</v>
       </c>
-      <c r="E20" s="100">
-        <v>2</v>
-      </c>
-      <c r="F20" s="101"/>
+      <c r="E20" s="81">
+        <v>3</v>
+      </c>
+      <c r="F20" s="83"/>
       <c r="G20" s="55"/>
       <c r="H20" s="53"/>
       <c r="I20" s="55"/>
-      <c r="J20" s="99" t="s">
-        <v>264</v>
-      </c>
-      <c r="K20" s="100">
+      <c r="J20" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="K20" s="81">
         <v>2</v>
       </c>
-      <c r="L20" s="100">
-        <v>3</v>
-      </c>
-      <c r="M20" s="101"/>
+      <c r="L20" s="81">
+        <v>2</v>
+      </c>
+      <c r="M20" s="83"/>
       <c r="N20" s="29"/>
       <c r="O20" s="1"/>
       <c r="P20" s="65"/>
@@ -11061,27 +11156,27 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
     </row>
-    <row r="21" spans="1:25" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="53"/>
       <c r="B21" s="55"/>
-      <c r="C21" s="101" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="101">
+      <c r="C21" s="83" t="s">
+        <v>252</v>
+      </c>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="83">
         <v>0.5</v>
       </c>
       <c r="G21" s="55"/>
       <c r="H21" s="53"/>
       <c r="I21" s="55"/>
-      <c r="J21" s="101" t="s">
-        <v>155</v>
-      </c>
-      <c r="K21" s="100"/>
-      <c r="L21" s="100"/>
-      <c r="M21" s="101">
-        <v>0.5</v>
+      <c r="J21" s="83" t="s">
+        <v>263</v>
+      </c>
+      <c r="K21" s="81"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="83">
+        <v>1</v>
       </c>
       <c r="N21" s="29"/>
       <c r="O21" s="1"/>
@@ -11098,27 +11193,27 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
-    <row r="22" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="53"/>
       <c r="B22" s="55"/>
-      <c r="C22" s="101" t="s">
-        <v>142</v>
-      </c>
-      <c r="D22" s="100"/>
-      <c r="E22" s="100"/>
-      <c r="F22" s="101">
+      <c r="C22" s="83" t="s">
+        <v>253</v>
+      </c>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="83">
         <v>0.5</v>
       </c>
       <c r="G22" s="55"/>
       <c r="H22" s="53"/>
       <c r="I22" s="55"/>
-      <c r="J22" s="101" t="s">
-        <v>265</v>
-      </c>
-      <c r="K22" s="100"/>
-      <c r="L22" s="100"/>
-      <c r="M22" s="101">
-        <v>0.5</v>
+      <c r="J22" s="83" t="s">
+        <v>264</v>
+      </c>
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="83">
+        <v>1</v>
       </c>
       <c r="N22" s="29"/>
       <c r="O22" s="1"/>
@@ -11133,27 +11228,27 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
     </row>
-    <row r="23" spans="1:25" s="48" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" s="48" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="53"/>
       <c r="B23" s="55"/>
-      <c r="C23" s="101" t="s">
-        <v>143</v>
-      </c>
-      <c r="D23" s="100"/>
-      <c r="E23" s="100"/>
-      <c r="F23" s="101">
+      <c r="C23" s="83" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="83">
         <v>0.5</v>
       </c>
       <c r="G23" s="55"/>
       <c r="H23" s="53"/>
       <c r="I23" s="55"/>
-      <c r="J23" s="101" t="s">
-        <v>156</v>
-      </c>
-      <c r="K23" s="100"/>
-      <c r="L23" s="100"/>
-      <c r="M23" s="101">
-        <v>0.5</v>
+      <c r="J23" s="83" t="s">
+        <v>266</v>
+      </c>
+      <c r="K23" s="81"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="83">
+        <v>1</v>
       </c>
       <c r="N23" s="29"/>
       <c r="O23" s="49"/>
@@ -11171,24 +11266,24 @@
     <row r="24" spans="1:25" s="48" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="53"/>
       <c r="B24" s="55"/>
-      <c r="C24" s="101" t="s">
-        <v>144</v>
-      </c>
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="101">
-        <v>0.5</v>
+      <c r="C24" s="83" t="s">
+        <v>254</v>
+      </c>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="83">
+        <v>1</v>
       </c>
       <c r="G24" s="55"/>
       <c r="H24" s="53"/>
       <c r="I24" s="55"/>
-      <c r="J24" s="101" t="s">
-        <v>157</v>
-      </c>
-      <c r="K24" s="100"/>
-      <c r="L24" s="100"/>
-      <c r="M24" s="101">
-        <v>0.5</v>
+      <c r="J24" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="K24" s="81"/>
+      <c r="L24" s="81"/>
+      <c r="M24" s="83">
+        <v>1</v>
       </c>
       <c r="N24" s="29"/>
       <c r="O24" s="49"/>
@@ -11206,21 +11301,21 @@
     <row r="25" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="53"/>
       <c r="B25" s="55"/>
-      <c r="C25" s="83"/>
+      <c r="C25" s="83" t="s">
+        <v>255</v>
+      </c>
       <c r="D25" s="81"/>
       <c r="E25" s="81"/>
-      <c r="F25" s="83"/>
+      <c r="F25" s="83">
+        <v>1</v>
+      </c>
       <c r="G25" s="55"/>
       <c r="H25" s="53"/>
       <c r="I25" s="55"/>
-      <c r="J25" s="101" t="s">
-        <v>160</v>
-      </c>
-      <c r="K25" s="100"/>
-      <c r="L25" s="100"/>
-      <c r="M25" s="101">
-        <v>2</v>
-      </c>
+      <c r="J25" s="83"/>
+      <c r="K25" s="81"/>
+      <c r="L25" s="81"/>
+      <c r="M25" s="83"/>
       <c r="N25" s="29"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -11237,22 +11332,26 @@
     <row r="26" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="53"/>
       <c r="B26" s="55"/>
-      <c r="C26" s="99" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="100">
-        <v>2</v>
-      </c>
-      <c r="E26" s="100">
+      <c r="C26" s="83" t="s">
+        <v>257</v>
+      </c>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="82">
         <v>1</v>
       </c>
-      <c r="F26" s="104"/>
       <c r="G26" s="55"/>
       <c r="H26" s="53"/>
       <c r="I26" s="55"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="81"/>
-      <c r="L26" s="81"/>
+      <c r="J26" s="80" t="s">
+        <v>248</v>
+      </c>
+      <c r="K26" s="81">
+        <v>2</v>
+      </c>
+      <c r="L26" s="81">
+        <v>2</v>
+      </c>
       <c r="M26" s="82"/>
       <c r="N26" s="29"/>
       <c r="O26" s="1"/>
@@ -11267,30 +11366,24 @@
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
     </row>
-    <row r="27" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="53"/>
       <c r="B27" s="55"/>
-      <c r="C27" s="101" t="s">
-        <v>174</v>
-      </c>
-      <c r="D27" s="100"/>
-      <c r="E27" s="100"/>
-      <c r="F27" s="104">
-        <v>0.5</v>
-      </c>
+      <c r="C27" s="83"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="82"/>
       <c r="G27" s="55"/>
       <c r="H27" s="53"/>
       <c r="I27" s="55"/>
-      <c r="J27" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="K27" s="81">
-        <v>2</v>
-      </c>
-      <c r="L27" s="81">
-        <v>2</v>
-      </c>
-      <c r="M27" s="83"/>
+      <c r="J27" s="83" t="s">
+        <v>271</v>
+      </c>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="83">
+        <v>0.5</v>
+      </c>
       <c r="N27" s="29"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -11304,27 +11397,29 @@
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
     </row>
-    <row r="28" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="53"/>
       <c r="B28" s="55"/>
-      <c r="C28" s="101" t="s">
-        <v>176</v>
-      </c>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="104">
-        <v>1</v>
-      </c>
+      <c r="C28" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="D28" s="81">
+        <v>2</v>
+      </c>
+      <c r="E28" s="81">
+        <v>3</v>
+      </c>
+      <c r="F28" s="82"/>
       <c r="G28" s="55"/>
       <c r="H28" s="53"/>
       <c r="I28" s="55"/>
-      <c r="J28" s="96" t="s">
-        <v>168</v>
+      <c r="J28" s="83" t="s">
+        <v>268</v>
       </c>
       <c r="K28" s="84"/>
       <c r="L28" s="84"/>
       <c r="M28" s="85">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N28" s="29"/>
       <c r="O28" s="1"/>
@@ -11342,19 +11437,19 @@
     <row r="29" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="53"/>
       <c r="B29" s="55"/>
-      <c r="C29" s="101" t="s">
-        <v>175</v>
-      </c>
-      <c r="D29" s="100"/>
-      <c r="E29" s="100"/>
-      <c r="F29" s="104">
-        <v>0.5</v>
+      <c r="C29" s="83" t="s">
+        <v>259</v>
+      </c>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="82">
+        <v>1</v>
       </c>
       <c r="G29" s="55"/>
       <c r="H29" s="53"/>
       <c r="I29" s="55"/>
-      <c r="J29" s="53" t="s">
-        <v>169</v>
+      <c r="J29" s="83" t="s">
+        <v>269</v>
       </c>
       <c r="K29" s="84"/>
       <c r="L29" s="84"/>
@@ -11374,23 +11469,27 @@
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
     </row>
-    <row r="30" spans="1:25" s="48" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" s="48" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="53"/>
       <c r="B30" s="55"/>
-      <c r="C30" s="83"/>
+      <c r="C30" s="83" t="s">
+        <v>260</v>
+      </c>
       <c r="D30" s="81"/>
       <c r="E30" s="81"/>
-      <c r="F30" s="82"/>
+      <c r="F30" s="82">
+        <v>1</v>
+      </c>
       <c r="G30" s="55"/>
       <c r="H30" s="53"/>
       <c r="I30" s="55"/>
-      <c r="J30" s="53" t="s">
-        <v>170</v>
+      <c r="J30" s="83" t="s">
+        <v>270</v>
       </c>
       <c r="K30" s="87"/>
       <c r="L30" s="87"/>
       <c r="M30" s="83">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="N30" s="29"/>
       <c r="O30" s="49"/>
@@ -11405,26 +11504,24 @@
       <c r="X30" s="49"/>
       <c r="Y30" s="49"/>
     </row>
-    <row r="31" spans="1:25" s="48" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" s="48" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="53"/>
       <c r="B31" s="55"/>
-      <c r="C31" s="99" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="100">
-        <v>2</v>
-      </c>
-      <c r="E31" s="100">
-        <v>2</v>
-      </c>
-      <c r="F31" s="104"/>
+      <c r="C31" s="83" t="s">
+        <v>261</v>
+      </c>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="82">
+        <v>0.5</v>
+      </c>
       <c r="G31" s="55"/>
       <c r="H31" s="53"/>
       <c r="I31" s="55"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="53"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="81"/>
+      <c r="L31" s="81"/>
+      <c r="M31" s="83"/>
       <c r="N31" s="29"/>
       <c r="O31" s="49"/>
       <c r="P31" s="49"/>
@@ -11441,21 +11538,27 @@
     <row r="32" spans="1:25" s="48" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="53"/>
       <c r="B32" s="55"/>
-      <c r="C32" s="101" t="s">
-        <v>161</v>
-      </c>
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="104">
+      <c r="C32" s="83" t="s">
+        <v>262</v>
+      </c>
+      <c r="D32" s="81"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="82">
         <v>0.5</v>
       </c>
       <c r="G32" s="55"/>
       <c r="H32" s="53"/>
       <c r="I32" s="55"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="53"/>
+      <c r="J32" s="54" t="s">
+        <v>249</v>
+      </c>
+      <c r="K32" s="81">
+        <v>2</v>
+      </c>
+      <c r="L32" s="81">
+        <v>2</v>
+      </c>
+      <c r="M32" s="83"/>
       <c r="N32" s="29"/>
       <c r="O32" s="49"/>
       <c r="P32" s="49"/>
@@ -11472,21 +11575,21 @@
     <row r="33" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="53"/>
       <c r="B33" s="55"/>
-      <c r="C33" s="101" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" s="100"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="104">
-        <v>1</v>
-      </c>
+      <c r="C33" s="83"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="82"/>
       <c r="G33" s="55"/>
       <c r="H33" s="53"/>
       <c r="I33" s="55"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="53"/>
+      <c r="J33" s="83" t="s">
+        <v>273</v>
+      </c>
+      <c r="K33" s="81"/>
+      <c r="L33" s="81"/>
+      <c r="M33" s="83">
+        <v>0.5</v>
+      </c>
       <c r="N33" s="29"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -11503,21 +11606,21 @@
     <row r="34" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="53"/>
       <c r="B34" s="55"/>
-      <c r="C34" s="101" t="s">
-        <v>165</v>
-      </c>
-      <c r="D34" s="100"/>
-      <c r="E34" s="100"/>
-      <c r="F34" s="104">
-        <v>1</v>
-      </c>
+      <c r="C34" s="83"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="82"/>
       <c r="G34" s="55"/>
       <c r="H34" s="53"/>
       <c r="I34" s="55"/>
-      <c r="J34" s="53"/>
+      <c r="J34" s="53" t="s">
+        <v>272</v>
+      </c>
       <c r="K34" s="58"/>
       <c r="L34" s="58"/>
-      <c r="M34" s="53"/>
+      <c r="M34" s="53">
+        <v>1</v>
+      </c>
       <c r="N34" s="29"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -11534,21 +11637,21 @@
     <row r="35" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="53"/>
       <c r="B35" s="55"/>
-      <c r="C35" s="101" t="s">
-        <v>163</v>
-      </c>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="104">
-        <v>1</v>
-      </c>
+      <c r="C35" s="83"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="82"/>
       <c r="G35" s="55"/>
       <c r="H35" s="53"/>
       <c r="I35" s="55"/>
-      <c r="J35" s="53"/>
+      <c r="J35" s="53" t="s">
+        <v>274</v>
+      </c>
       <c r="K35" s="58"/>
       <c r="L35" s="58"/>
-      <c r="M35" s="53"/>
+      <c r="M35" s="53">
+        <v>1</v>
+      </c>
       <c r="N35" s="29"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -11562,24 +11665,24 @@
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
     </row>
-    <row r="36" spans="1:25" s="48" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" s="48" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="53"/>
       <c r="B36" s="55"/>
-      <c r="C36" s="101" t="s">
-        <v>164</v>
-      </c>
-      <c r="D36" s="100"/>
-      <c r="E36" s="100"/>
-      <c r="F36" s="104">
-        <v>1</v>
-      </c>
+      <c r="C36" s="83"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="82"/>
       <c r="G36" s="55"/>
       <c r="H36" s="53"/>
       <c r="I36" s="55"/>
-      <c r="J36" s="53"/>
+      <c r="J36" s="53" t="s">
+        <v>276</v>
+      </c>
       <c r="K36" s="58"/>
       <c r="L36" s="58"/>
-      <c r="M36" s="53"/>
+      <c r="M36" s="53">
+        <v>1</v>
+      </c>
       <c r="N36" s="29"/>
       <c r="O36" s="49"/>
       <c r="P36" s="49"/>
@@ -11630,7 +11733,7 @@
       <c r="E38" s="56"/>
       <c r="F38" s="56">
         <f>SUM(F20:F37)</f>
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="G38" s="55"/>
       <c r="H38" s="53"/>
@@ -11642,7 +11745,7 @@
       <c r="L38" s="56"/>
       <c r="M38" s="56">
         <f>SUM(M20:M37)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="N38" s="29"/>
       <c r="O38" s="1"/>
@@ -11661,15 +11764,15 @@
       <c r="A39" s="53"/>
       <c r="B39" s="55"/>
       <c r="C39" s="55"/>
-      <c r="D39" s="143"/>
-      <c r="E39" s="144"/>
+      <c r="D39" s="140"/>
+      <c r="E39" s="141"/>
       <c r="F39" s="55"/>
       <c r="G39" s="55"/>
       <c r="H39" s="53"/>
       <c r="I39" s="55"/>
       <c r="J39" s="55"/>
-      <c r="K39" s="143"/>
-      <c r="L39" s="144"/>
+      <c r="K39" s="140"/>
+      <c r="L39" s="141"/>
       <c r="M39" s="55"/>
       <c r="N39" s="29"/>
       <c r="O39" s="1"/>
@@ -13421,7 +13524,7 @@
       <c r="C12" s="67"/>
       <c r="E12" s="67"/>
       <c r="F12" s="68" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="G12" s="67"/>
       <c r="H12" s="68" t="s">
@@ -13526,11 +13629,11 @@
       <c r="D19" s="67"/>
       <c r="E19" s="67"/>
       <c r="F19" s="74" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="G19" s="67"/>
       <c r="H19" s="68" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="I19" s="67"/>
       <c r="J19" s="67"/>
@@ -13546,7 +13649,7 @@
       </c>
       <c r="G20" s="67"/>
       <c r="H20" s="74" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="I20" s="67"/>
       <c r="J20" s="67"/>
@@ -13561,8 +13664,8 @@
         <v>109</v>
       </c>
       <c r="G21" s="67"/>
-      <c r="H21" s="102" t="s">
-        <v>179</v>
+      <c r="H21" s="98" t="s">
+        <v>157</v>
       </c>
       <c r="I21" s="67"/>
       <c r="J21" s="67"/>
@@ -13577,7 +13680,7 @@
       </c>
       <c r="G22" s="67"/>
       <c r="H22" s="74" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="I22" s="67"/>
       <c r="J22" s="67"/>
@@ -13724,7 +13827,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13739,45 +13842,45 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="90" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="63"/>
       <c r="B2" s="64" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="92"/>
       <c r="B3" s="93" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="65"/>
       <c r="B4" s="64" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="66"/>
       <c r="B5" s="64" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D6" s="89" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E6" s="89" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G6" s="89" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H6" s="89" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
@@ -13785,61 +13888,91 @@
         <v>73</v>
       </c>
       <c r="E7" s="94" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="G7" s="88" t="s">
         <v>72</v>
       </c>
       <c r="H7" s="91" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="D8" s="88" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E8" s="95" t="s">
-        <v>159</v>
+        <v>151</v>
+      </c>
+      <c r="G8" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" s="143" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="D9" s="79" t="s">
-        <v>172</v>
-      </c>
-      <c r="E9" s="98" t="s">
-        <v>173</v>
+        <v>153</v>
+      </c>
+      <c r="E9" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="G9" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="H9" s="144" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="D10" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="106" t="s">
-        <v>184</v>
+      <c r="E10" s="101" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="97" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="D11" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="106" t="s">
-        <v>185</v>
+      <c r="E11" s="101" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="122" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11" s="144" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="D12" s="88" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="E12" s="91" t="s">
-        <v>187</v>
+        <v>165</v>
+      </c>
+      <c r="G12" s="122" t="s">
+        <v>192</v>
+      </c>
+      <c r="H12" s="91" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="D13" s="88" t="s">
-        <v>261</v>
-      </c>
-      <c r="E13" s="106" t="s">
-        <v>262</v>
+        <v>239</v>
+      </c>
+      <c r="E13" s="101" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -13866,493 +13999,493 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="69.75" x14ac:dyDescent="0.35">
-      <c r="A1" s="124" t="s">
-        <v>257</v>
-      </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
+      <c r="A1" s="119" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
     </row>
     <row r="2" spans="1:13" ht="37.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="102" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="102" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="102" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="103" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="104" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="105"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="107" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="108" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="109" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="105"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="110" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="111" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="109" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="105"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="105"/>
+    </row>
+    <row r="6" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="112" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="106"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="113" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="105" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="106" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="113" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="105" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="106" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="113" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" s="105" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="106" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="114" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="105"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="113" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="105" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" s="106" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="D11" s="111"/>
+      <c r="E11" s="105"/>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="113" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="107" t="s">
+      <c r="B12" s="105" t="s">
         <v>190</v>
       </c>
-      <c r="D2" s="108" t="s">
+      <c r="C12" s="106" t="s">
         <v>191</v>
       </c>
-      <c r="E2" s="109" t="s">
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+    </row>
+    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="105"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="109" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="110"/>
-      <c r="B3" s="110"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="112" t="s">
+      <c r="B14" s="105"/>
+      <c r="C14" s="106"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="E3" s="113" t="s">
+      <c r="B15" s="105"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+    </row>
+    <row r="16" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="112" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="114" t="s">
+      <c r="B16" s="105" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="110"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="115" t="s">
+      <c r="C16" s="106"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+    </row>
+    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="104" t="s">
         <v>196</v>
       </c>
-      <c r="E4" s="116" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="114" t="s">
+      <c r="B17" s="105" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="110"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="110"/>
-    </row>
-    <row r="6" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="117" t="s">
+      <c r="C17" s="106"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="113" t="s">
         <v>198</v>
       </c>
-      <c r="B6" s="110" t="s">
+      <c r="B18" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="111"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="118" t="s">
+      <c r="C18" s="106" t="s">
         <v>200</v>
       </c>
-      <c r="B7" s="110" t="s">
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="113" t="s">
         <v>201</v>
       </c>
-      <c r="C7" s="111" t="s">
+      <c r="B19" s="105" t="s">
+        <v>199</v>
+      </c>
+      <c r="C19" s="106" t="s">
         <v>202</v>
       </c>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-    </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="118" t="s">
+      <c r="D19" s="105"/>
+      <c r="E19" s="105"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A20" s="113" t="s">
         <v>203</v>
       </c>
-      <c r="B8" s="110" t="s">
+      <c r="B20" s="105" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" s="106" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20" s="105"/>
+      <c r="E20" s="105"/>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="113" t="s">
         <v>204</v>
       </c>
-      <c r="C8" s="111" t="s">
-        <v>202</v>
-      </c>
-      <c r="D8" s="110"/>
-      <c r="E8" s="110"/>
-    </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="118" t="s">
+      <c r="B21" s="105" t="s">
         <v>205</v>
       </c>
-      <c r="B9" s="110" t="s">
+      <c r="C21" s="106" t="s">
         <v>206</v>
       </c>
-      <c r="C9" s="111" t="s">
-        <v>202</v>
-      </c>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="119" t="s">
+      <c r="D21" s="105"/>
+      <c r="E21" s="105"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A22" s="113" t="s">
         <v>207</v>
       </c>
-      <c r="B10" s="110"/>
-      <c r="C10" s="111"/>
-      <c r="D10" s="110"/>
-      <c r="E10" s="110"/>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="118" t="s">
+      <c r="B22" s="105" t="s">
         <v>208</v>
       </c>
-      <c r="B11" s="110" t="s">
+      <c r="C22" s="106" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="113"/>
+      <c r="B23" s="105"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="114" t="s">
         <v>209</v>
       </c>
-      <c r="C11" s="111" t="s">
+      <c r="B24" s="105"/>
+      <c r="C24" s="106"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A25" s="113" t="s">
         <v>210</v>
       </c>
-      <c r="D11" s="116"/>
-      <c r="E11" s="110"/>
-    </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="118" t="s">
+      <c r="B25" s="105" t="s">
         <v>211</v>
       </c>
-      <c r="B12" s="110" t="s">
+      <c r="C25" s="106" t="s">
+        <v>180</v>
+      </c>
+      <c r="D25" s="105"/>
+      <c r="E25" s="105"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="114"/>
+      <c r="B26" s="105"/>
+      <c r="C26" s="106"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="105"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="115" t="s">
         <v>212</v>
       </c>
-      <c r="C12" s="111" t="s">
+      <c r="B27" s="105"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="113" t="s">
         <v>213</v>
       </c>
-      <c r="D12" s="110"/>
-      <c r="E12" s="110"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="110"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="114" t="s">
+      <c r="B28" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="106"/>
+      <c r="D28" s="105"/>
+      <c r="E28" s="105"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="113" t="s">
         <v>214</v>
       </c>
-      <c r="B14" s="110"/>
-      <c r="C14" s="111"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="120" t="s">
+      <c r="B29" s="105" t="s">
         <v>215</v>
       </c>
-      <c r="B15" s="110"/>
-      <c r="C15" s="111"/>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-    </row>
-    <row r="16" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="117" t="s">
+      <c r="C29" s="106"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="105"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="113" t="s">
         <v>216</v>
       </c>
-      <c r="B16" s="110" t="s">
+      <c r="B30" s="105" t="s">
         <v>217</v>
       </c>
-      <c r="C16" s="111"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-    </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="109" t="s">
+      <c r="C30" s="106"/>
+      <c r="D30" s="105"/>
+      <c r="E30" s="105"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="113" t="s">
         <v>218</v>
       </c>
-      <c r="B17" s="110" t="s">
+      <c r="B31" s="105" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="111"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="110"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="118" t="s">
+      <c r="C31" s="106"/>
+      <c r="D31" s="105"/>
+      <c r="E31" s="105"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="105"/>
+      <c r="B32" s="105"/>
+      <c r="C32" s="106"/>
+      <c r="D32" s="105"/>
+      <c r="E32" s="105"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="114" t="s">
         <v>220</v>
       </c>
-      <c r="B18" s="110" t="s">
+      <c r="B33" s="105"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="105"/>
+      <c r="E33" s="105"/>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A34" s="113" t="s">
         <v>221</v>
       </c>
-      <c r="C18" s="111" t="s">
+      <c r="B34" s="105" t="s">
         <v>222</v>
       </c>
-      <c r="D18" s="110"/>
-      <c r="E18" s="110"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="118" t="s">
+      <c r="C34" s="106" t="s">
+        <v>188</v>
+      </c>
+      <c r="D34" s="105"/>
+      <c r="E34" s="105"/>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A35" s="113" t="s">
+        <v>236</v>
+      </c>
+      <c r="B35" s="105" t="s">
         <v>223</v>
       </c>
-      <c r="B19" s="110" t="s">
-        <v>221</v>
-      </c>
-      <c r="C19" s="111" t="s">
+      <c r="C35" s="106" t="s">
+        <v>226</v>
+      </c>
+      <c r="D35" s="105"/>
+      <c r="E35" s="105"/>
+    </row>
+    <row r="36" spans="1:5" s="96" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A36" s="113" t="s">
+        <v>237</v>
+      </c>
+      <c r="B36" s="105" t="s">
+        <v>223</v>
+      </c>
+      <c r="C36" s="106" t="s">
+        <v>226</v>
+      </c>
+      <c r="D36" s="105"/>
+      <c r="E36" s="105"/>
+    </row>
+    <row r="37" spans="1:5" s="96" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A37" s="113" t="s">
+        <v>238</v>
+      </c>
+      <c r="B37" s="105" t="s">
+        <v>223</v>
+      </c>
+      <c r="C37" s="106" t="s">
+        <v>226</v>
+      </c>
+      <c r="D37" s="105"/>
+      <c r="E37" s="105"/>
+    </row>
+    <row r="38" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="113" t="s">
         <v>224</v>
       </c>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="118" t="s">
+      <c r="B38" s="105" t="s">
         <v>225</v>
       </c>
-      <c r="B20" s="110" t="s">
-        <v>221</v>
-      </c>
-      <c r="C20" s="111" t="s">
-        <v>224</v>
-      </c>
-      <c r="D20" s="110"/>
-      <c r="E20" s="110"/>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="118" t="s">
+      <c r="C38" s="106" t="s">
         <v>226</v>
       </c>
-      <c r="B21" s="110" t="s">
+      <c r="D38" s="116"/>
+      <c r="E38" s="116"/>
+    </row>
+    <row r="39" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="113" t="s">
         <v>227</v>
       </c>
-      <c r="C21" s="111" t="s">
+      <c r="B39" s="105" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="110"/>
-      <c r="E21" s="110"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" s="118" t="s">
+      <c r="C39" s="106" t="s">
+        <v>226</v>
+      </c>
+      <c r="D39" s="105"/>
+      <c r="E39" s="105"/>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A40" s="113" t="s">
         <v>229</v>
       </c>
-      <c r="B22" s="110" t="s">
+      <c r="B40" s="105" t="s">
         <v>230</v>
       </c>
-      <c r="C22" s="111" t="s">
-        <v>213</v>
-      </c>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="118"/>
-      <c r="B23" s="110"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="110"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="119" t="s">
+      <c r="C40" s="106" t="s">
+        <v>226</v>
+      </c>
+      <c r="D40" s="105"/>
+      <c r="E40" s="105"/>
+    </row>
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="105"/>
+      <c r="B41" s="105"/>
+      <c r="C41" s="106"/>
+      <c r="D41" s="105"/>
+      <c r="E41" s="105"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="114" t="s">
         <v>231</v>
       </c>
-      <c r="B24" s="110"/>
-      <c r="C24" s="111"/>
-      <c r="D24" s="110"/>
-      <c r="E24" s="110"/>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="118" t="s">
+      <c r="B42" s="105"/>
+      <c r="C42" s="106"/>
+      <c r="D42" s="105"/>
+      <c r="E42" s="105"/>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" s="113" t="s">
         <v>232</v>
       </c>
-      <c r="B25" s="110" t="s">
+      <c r="B43" s="105" t="s">
         <v>233</v>
       </c>
-      <c r="C25" s="111" t="s">
-        <v>202</v>
-      </c>
-      <c r="D25" s="110"/>
-      <c r="E25" s="110"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="119"/>
-      <c r="B26" s="110"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="110"/>
-      <c r="E26" s="110"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="120" t="s">
+      <c r="C43" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="B27" s="110"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="118" t="s">
-        <v>235</v>
-      </c>
-      <c r="B28" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="111"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="110"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="118" t="s">
-        <v>236</v>
-      </c>
-      <c r="B29" s="110" t="s">
-        <v>237</v>
-      </c>
-      <c r="C29" s="111"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="110"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="118" t="s">
-        <v>238</v>
-      </c>
-      <c r="B30" s="110" t="s">
-        <v>239</v>
-      </c>
-      <c r="C30" s="111"/>
-      <c r="D30" s="110"/>
-      <c r="E30" s="110"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="118" t="s">
-        <v>240</v>
-      </c>
-      <c r="B31" s="110" t="s">
-        <v>241</v>
-      </c>
-      <c r="C31" s="111"/>
-      <c r="D31" s="110"/>
-      <c r="E31" s="110"/>
-    </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="110"/>
-      <c r="B32" s="110"/>
-      <c r="C32" s="111"/>
-      <c r="D32" s="110"/>
-      <c r="E32" s="110"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="119" t="s">
-        <v>242</v>
-      </c>
-      <c r="B33" s="110"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="110"/>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="118" t="s">
-        <v>243</v>
-      </c>
-      <c r="B34" s="110" t="s">
-        <v>244</v>
-      </c>
-      <c r="C34" s="111" t="s">
-        <v>210</v>
-      </c>
-      <c r="D34" s="110"/>
-      <c r="E34" s="110"/>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" s="118" t="s">
-        <v>258</v>
-      </c>
-      <c r="B35" s="110" t="s">
-        <v>245</v>
-      </c>
-      <c r="C35" s="111" t="s">
-        <v>248</v>
-      </c>
-      <c r="D35" s="110"/>
-      <c r="E35" s="110"/>
-    </row>
-    <row r="36" spans="1:5" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="118" t="s">
-        <v>259</v>
-      </c>
-      <c r="B36" s="110" t="s">
-        <v>245</v>
-      </c>
-      <c r="C36" s="111" t="s">
-        <v>248</v>
-      </c>
-      <c r="D36" s="110"/>
-      <c r="E36" s="110"/>
-    </row>
-    <row r="37" spans="1:5" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A37" s="118" t="s">
-        <v>260</v>
-      </c>
-      <c r="B37" s="110" t="s">
-        <v>245</v>
-      </c>
-      <c r="C37" s="111" t="s">
-        <v>248</v>
-      </c>
-      <c r="D37" s="110"/>
-      <c r="E37" s="110"/>
-    </row>
-    <row r="38" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="118" t="s">
-        <v>246</v>
-      </c>
-      <c r="B38" s="110" t="s">
-        <v>247</v>
-      </c>
-      <c r="C38" s="111" t="s">
-        <v>248</v>
-      </c>
-      <c r="D38" s="121"/>
-      <c r="E38" s="121"/>
-    </row>
-    <row r="39" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="118" t="s">
-        <v>249</v>
-      </c>
-      <c r="B39" s="110" t="s">
-        <v>250</v>
-      </c>
-      <c r="C39" s="111" t="s">
-        <v>248</v>
-      </c>
-      <c r="D39" s="110"/>
-      <c r="E39" s="110"/>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A40" s="118" t="s">
-        <v>251</v>
-      </c>
-      <c r="B40" s="110" t="s">
-        <v>252</v>
-      </c>
-      <c r="C40" s="111" t="s">
-        <v>248</v>
-      </c>
-      <c r="D40" s="110"/>
-      <c r="E40" s="110"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="110"/>
-      <c r="B41" s="110"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="110"/>
-      <c r="E41" s="110"/>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="119" t="s">
-        <v>253</v>
-      </c>
-      <c r="B42" s="110"/>
-      <c r="C42" s="111"/>
-      <c r="D42" s="110"/>
-      <c r="E42" s="110"/>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" s="118" t="s">
-        <v>254</v>
-      </c>
-      <c r="B43" s="110" t="s">
-        <v>255</v>
-      </c>
-      <c r="C43" s="111" t="s">
-        <v>256</v>
-      </c>
-      <c r="D43" s="110"/>
-      <c r="E43" s="110"/>
+      <c r="D43" s="105"/>
+      <c r="E43" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
last details for alpha
Added icon and splash screen
</commit_message>
<xml_diff>
--- a/BacklogTasks.xlsx
+++ b/BacklogTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnityProjects\DesignAndPublishUnity\CoreRun\CoreRun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE69B5C-FEEA-46BC-8DA7-E07ABA4E1E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14F63F5-9020-4CDD-B61D-2052D6E027D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13950" yWindow="75" windowWidth="14715" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="205">
   <si>
     <t>Area</t>
   </si>
@@ -647,6 +647,12 @@
   </si>
   <si>
     <t>Obstacle 5</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Add ability to regain lives after layers</t>
   </si>
 </sst>
 </file>
@@ -1907,8 +1913,8 @@
   </sheetPr>
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2281,7 +2287,9 @@
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="A15" s="18" t="s">
+        <v>203</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2326,7 +2334,9 @@
     </row>
     <row r="17" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -15159,7 +15169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDD8067-A579-4749-B3F6-18055CAB8E07}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Preperation for PC release
Made minor fixes in preparation for PC release.
</commit_message>
<xml_diff>
--- a/BacklogTasks.xlsx
+++ b/BacklogTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnityProjects\DesignAndPublishUnity\CoreRun\CoreRun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14F63F5-9020-4CDD-B61D-2052D6E027D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2994ABC-9C33-489D-89C0-E0FDA5079436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="75" windowWidth="14715" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13950" yWindow="75" windowWidth="14715" windowHeight="15495" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="205">
   <si>
     <t>Area</t>
   </si>
@@ -490,9 +490,6 @@
     <t>The character squinches his eyes when he is shrinking</t>
   </si>
   <si>
-    <t>Enemies appear on the main menu occasionally</t>
-  </si>
-  <si>
     <t>Shrinking ability is limited by a resource on a bar</t>
   </si>
   <si>
@@ -589,9 +586,6 @@
     <t>monster_mini_cutie_battle_6.wav</t>
   </si>
   <si>
-    <t>Facts about Coren appear on the menu occasionally</t>
-  </si>
-  <si>
     <t>There's a large pink enemy that blocks the player with its' eyes</t>
   </si>
   <si>
@@ -619,9 +613,6 @@
     <t>There's a popup when the Layer Transitions instead of a cave</t>
   </si>
   <si>
-    <t>There is a credits section on the main menu that thanks the different asset providers from the Unity Store</t>
-  </si>
-  <si>
     <t>ForestFloorGreen.png</t>
   </si>
   <si>
@@ -652,7 +643,16 @@
     <t>Distribution</t>
   </si>
   <si>
-    <t>Add ability to regain lives after layers</t>
+    <t>There is a credits section on the page the game is available, thanking the different asset providers.</t>
+  </si>
+  <si>
+    <t>Player's regain lives after layers</t>
+  </si>
+  <si>
+    <t>Player's on touch devices can move with touch controls</t>
+  </si>
+  <si>
+    <t>The main menu is simple and has a nice graphic</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1441,6 +1441,9 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1481,6 +1484,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1913,8 +1922,8 @@
   </sheetPr>
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1933,14 +1942,14 @@
       <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="117" t="s">
+      <c r="C1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="118"/>
-      <c r="E1" s="117" t="s">
+      <c r="D1" s="119"/>
+      <c r="E1" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="119"/>
+      <c r="F1" s="120"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1959,14 +1968,14 @@
     <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="120" t="s">
+      <c r="C2" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="118"/>
-      <c r="E2" s="120" t="s">
+      <c r="D2" s="119"/>
+      <c r="E2" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="119"/>
+      <c r="F2" s="120"/>
       <c r="G2" s="31"/>
       <c r="H2" s="30" t="s">
         <v>73</v>
@@ -1987,14 +1996,14 @@
     <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="118"/>
-      <c r="E3" s="120" t="s">
+      <c r="D3" s="119"/>
+      <c r="E3" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="119"/>
+      <c r="F3" s="120"/>
       <c r="G3" s="82"/>
       <c r="H3" s="30"/>
       <c r="I3" s="1"/>
@@ -2013,14 +2022,14 @@
     <row r="4" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="114" t="s">
+      <c r="C4" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="115"/>
-      <c r="E4" s="114" t="s">
+      <c r="D4" s="116"/>
+      <c r="E4" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="116"/>
+      <c r="F4" s="117"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2180,18 +2189,12 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1">
-        <v>2</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
       <c r="H11" s="1"/>
@@ -2208,18 +2211,12 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1">
-        <v>3</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
       <c r="H12" s="1"/>
@@ -2239,7 +2236,7 @@
     <row r="13" spans="1:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -2288,7 +2285,7 @@
     </row>
     <row r="15" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2334,12 +2331,16 @@
     </row>
     <row r="17" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C17" s="1"/>
+      <c r="B17" s="129" t="s">
+        <v>202</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
       <c r="H17" s="1"/>
@@ -2356,12 +2357,18 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="129" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>3</v>
+      </c>
       <c r="F18" s="8"/>
       <c r="G18" s="9"/>
       <c r="H18" s="1"/>
@@ -2378,12 +2385,18 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B19" s="129" t="s">
+        <v>204</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>3</v>
+      </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
       <c r="H19" s="1"/>
@@ -3740,11 +3753,11 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="124" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -3896,7 +3909,7 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="126" t="s">
+      <c r="A9" s="127" t="s">
         <v>141</v>
       </c>
       <c r="B9" s="1"/>
@@ -3931,7 +3944,7 @@
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="127"/>
+      <c r="A10" s="128"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="19" t="s">
@@ -3964,7 +3977,7 @@
       <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="127"/>
+      <c r="A11" s="128"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="19" t="s">
@@ -4092,104 +4105,104 @@
       <c r="Y14" s="1"/>
     </row>
     <row r="15" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="124"/>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="118"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="118"/>
-      <c r="M15" s="118"/>
-      <c r="N15" s="118"/>
-      <c r="O15" s="118"/>
-      <c r="P15" s="118"/>
-      <c r="Q15" s="118"/>
-      <c r="R15" s="118"/>
-      <c r="S15" s="118"/>
-      <c r="T15" s="118"/>
-      <c r="U15" s="118"/>
-      <c r="V15" s="118"/>
-      <c r="W15" s="118"/>
-      <c r="X15" s="118"/>
-      <c r="Y15" s="118"/>
+      <c r="A15" s="125"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="119"/>
+      <c r="L15" s="119"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="119"/>
+      <c r="P15" s="119"/>
+      <c r="Q15" s="119"/>
+      <c r="R15" s="119"/>
+      <c r="S15" s="119"/>
+      <c r="T15" s="119"/>
+      <c r="U15" s="119"/>
+      <c r="V15" s="119"/>
+      <c r="W15" s="119"/>
+      <c r="X15" s="119"/>
+      <c r="Y15" s="119"/>
     </row>
     <row r="16" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="118"/>
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="118"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="118"/>
-      <c r="P16" s="118"/>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="118"/>
-      <c r="S16" s="118"/>
-      <c r="T16" s="118"/>
-      <c r="U16" s="118"/>
-      <c r="V16" s="118"/>
-      <c r="W16" s="118"/>
-      <c r="X16" s="118"/>
-      <c r="Y16" s="118"/>
+      <c r="A16" s="119"/>
+      <c r="B16" s="119"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="119"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="119"/>
+      <c r="H16" s="119"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
+      <c r="M16" s="119"/>
+      <c r="N16" s="119"/>
+      <c r="O16" s="119"/>
+      <c r="P16" s="119"/>
+      <c r="Q16" s="119"/>
+      <c r="R16" s="119"/>
+      <c r="S16" s="119"/>
+      <c r="T16" s="119"/>
+      <c r="U16" s="119"/>
+      <c r="V16" s="119"/>
+      <c r="W16" s="119"/>
+      <c r="X16" s="119"/>
+      <c r="Y16" s="119"/>
     </row>
     <row r="17" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="118"/>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="118"/>
-      <c r="K17" s="118"/>
-      <c r="L17" s="118"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118"/>
-      <c r="O17" s="118"/>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="118"/>
-      <c r="S17" s="118"/>
-      <c r="T17" s="118"/>
-      <c r="U17" s="118"/>
-      <c r="V17" s="118"/>
-      <c r="W17" s="118"/>
-      <c r="X17" s="118"/>
-      <c r="Y17" s="118"/>
+      <c r="A17" s="119"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
+      <c r="M17" s="119"/>
+      <c r="N17" s="119"/>
+      <c r="O17" s="119"/>
+      <c r="P17" s="119"/>
+      <c r="Q17" s="119"/>
+      <c r="R17" s="119"/>
+      <c r="S17" s="119"/>
+      <c r="T17" s="119"/>
+      <c r="U17" s="119"/>
+      <c r="V17" s="119"/>
+      <c r="W17" s="119"/>
+      <c r="X17" s="119"/>
+      <c r="Y17" s="119"/>
     </row>
     <row r="18" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23"/>
       <c r="B18" s="24"/>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="122"/>
-      <c r="E18" s="122"/>
-      <c r="F18" s="122"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
       <c r="G18" s="24"/>
       <c r="H18" s="23"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="125" t="s">
+      <c r="J18" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="122"/>
-      <c r="L18" s="122"/>
-      <c r="M18" s="122"/>
+      <c r="K18" s="123"/>
+      <c r="L18" s="123"/>
+      <c r="M18" s="123"/>
       <c r="N18" s="13"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -4326,7 +4339,7 @@
       <c r="A22" s="23"/>
       <c r="B22" s="24"/>
       <c r="C22" s="89" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D22" s="90">
         <v>1</v>
@@ -4431,7 +4444,7 @@
       <c r="A25" s="23"/>
       <c r="B25" s="24"/>
       <c r="C25" s="89" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D25" s="90">
         <v>2</v>
@@ -4466,7 +4479,7 @@
       <c r="A26" s="23"/>
       <c r="B26" s="24"/>
       <c r="C26" s="89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D26" s="90">
         <v>2</v>
@@ -4501,7 +4514,7 @@
       <c r="A27" s="23"/>
       <c r="B27" s="24"/>
       <c r="C27" s="89" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D27" s="90">
         <v>2</v>
@@ -4571,7 +4584,7 @@
       <c r="A29" s="23"/>
       <c r="B29" s="24"/>
       <c r="C29" s="89" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D29" s="90">
         <v>3</v>
@@ -4859,15 +4872,15 @@
       <c r="A39" s="23"/>
       <c r="B39" s="24"/>
       <c r="C39" s="24"/>
-      <c r="D39" s="121"/>
-      <c r="E39" s="122"/>
+      <c r="D39" s="122"/>
+      <c r="E39" s="123"/>
       <c r="F39" s="24"/>
       <c r="G39" s="24"/>
       <c r="H39" s="23"/>
       <c r="I39" s="24"/>
       <c r="J39" s="24"/>
-      <c r="K39" s="121"/>
-      <c r="L39" s="122"/>
+      <c r="K39" s="122"/>
+      <c r="L39" s="123"/>
       <c r="M39" s="24"/>
       <c r="N39" s="13"/>
       <c r="O39" s="1"/>
@@ -6551,11 +6564,11 @@
       <c r="A4" s="77"/>
       <c r="B4" s="77"/>
       <c r="C4" s="77"/>
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="124" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
       <c r="G4" s="77"/>
       <c r="H4" s="77"/>
       <c r="I4" s="77"/>
@@ -6901,104 +6914,104 @@
       <c r="Y14" s="77"/>
     </row>
     <row r="15" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="124"/>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="118"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="118"/>
-      <c r="M15" s="118"/>
-      <c r="N15" s="118"/>
-      <c r="O15" s="118"/>
-      <c r="P15" s="118"/>
-      <c r="Q15" s="118"/>
-      <c r="R15" s="118"/>
-      <c r="S15" s="118"/>
-      <c r="T15" s="118"/>
-      <c r="U15" s="118"/>
-      <c r="V15" s="118"/>
-      <c r="W15" s="118"/>
-      <c r="X15" s="118"/>
-      <c r="Y15" s="118"/>
+      <c r="A15" s="125"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="119"/>
+      <c r="L15" s="119"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="119"/>
+      <c r="P15" s="119"/>
+      <c r="Q15" s="119"/>
+      <c r="R15" s="119"/>
+      <c r="S15" s="119"/>
+      <c r="T15" s="119"/>
+      <c r="U15" s="119"/>
+      <c r="V15" s="119"/>
+      <c r="W15" s="119"/>
+      <c r="X15" s="119"/>
+      <c r="Y15" s="119"/>
     </row>
     <row r="16" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="118"/>
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="118"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="118"/>
-      <c r="P16" s="118"/>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="118"/>
-      <c r="S16" s="118"/>
-      <c r="T16" s="118"/>
-      <c r="U16" s="118"/>
-      <c r="V16" s="118"/>
-      <c r="W16" s="118"/>
-      <c r="X16" s="118"/>
-      <c r="Y16" s="118"/>
+      <c r="A16" s="119"/>
+      <c r="B16" s="119"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="119"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="119"/>
+      <c r="H16" s="119"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
+      <c r="M16" s="119"/>
+      <c r="N16" s="119"/>
+      <c r="O16" s="119"/>
+      <c r="P16" s="119"/>
+      <c r="Q16" s="119"/>
+      <c r="R16" s="119"/>
+      <c r="S16" s="119"/>
+      <c r="T16" s="119"/>
+      <c r="U16" s="119"/>
+      <c r="V16" s="119"/>
+      <c r="W16" s="119"/>
+      <c r="X16" s="119"/>
+      <c r="Y16" s="119"/>
     </row>
     <row r="17" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="118"/>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="118"/>
-      <c r="K17" s="118"/>
-      <c r="L17" s="118"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118"/>
-      <c r="O17" s="118"/>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="118"/>
-      <c r="S17" s="118"/>
-      <c r="T17" s="118"/>
-      <c r="U17" s="118"/>
-      <c r="V17" s="118"/>
-      <c r="W17" s="118"/>
-      <c r="X17" s="118"/>
-      <c r="Y17" s="118"/>
+      <c r="A17" s="119"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
+      <c r="M17" s="119"/>
+      <c r="N17" s="119"/>
+      <c r="O17" s="119"/>
+      <c r="P17" s="119"/>
+      <c r="Q17" s="119"/>
+      <c r="R17" s="119"/>
+      <c r="S17" s="119"/>
+      <c r="T17" s="119"/>
+      <c r="U17" s="119"/>
+      <c r="V17" s="119"/>
+      <c r="W17" s="119"/>
+      <c r="X17" s="119"/>
+      <c r="Y17" s="119"/>
     </row>
     <row r="18" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23"/>
       <c r="B18" s="24"/>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="122"/>
-      <c r="E18" s="122"/>
-      <c r="F18" s="122"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
       <c r="G18" s="24"/>
       <c r="H18" s="23"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="125" t="s">
+      <c r="J18" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="122"/>
-      <c r="L18" s="122"/>
-      <c r="M18" s="122"/>
+      <c r="K18" s="123"/>
+      <c r="L18" s="123"/>
+      <c r="M18" s="123"/>
       <c r="N18" s="13"/>
       <c r="O18" s="77"/>
       <c r="P18" s="77"/>
@@ -7090,7 +7103,7 @@
       <c r="A21" s="23"/>
       <c r="B21" s="24"/>
       <c r="C21" s="89" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D21" s="90">
         <v>1</v>
@@ -7127,7 +7140,7 @@
       <c r="A22" s="23"/>
       <c r="B22" s="24"/>
       <c r="C22" s="89" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D22" s="90">
         <v>1</v>
@@ -7232,7 +7245,7 @@
       <c r="A25" s="23"/>
       <c r="B25" s="24"/>
       <c r="C25" s="89" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D25" s="90">
         <v>2</v>
@@ -7267,7 +7280,7 @@
       <c r="A26" s="23"/>
       <c r="B26" s="24"/>
       <c r="C26" s="89" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D26" s="90">
         <v>2</v>
@@ -7302,7 +7315,7 @@
       <c r="A27" s="23"/>
       <c r="B27" s="24"/>
       <c r="C27" s="89" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D27" s="90">
         <v>3</v>
@@ -7337,7 +7350,7 @@
       <c r="A28" s="23"/>
       <c r="B28" s="24"/>
       <c r="C28" s="89" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D28" s="90">
         <v>3</v>
@@ -7652,15 +7665,15 @@
       <c r="A39" s="23"/>
       <c r="B39" s="24"/>
       <c r="C39" s="24"/>
-      <c r="D39" s="121"/>
-      <c r="E39" s="122"/>
+      <c r="D39" s="122"/>
+      <c r="E39" s="123"/>
       <c r="F39" s="24"/>
       <c r="G39" s="24"/>
       <c r="H39" s="23"/>
       <c r="I39" s="24"/>
       <c r="J39" s="24"/>
-      <c r="K39" s="121"/>
-      <c r="L39" s="122"/>
+      <c r="K39" s="122"/>
+      <c r="L39" s="123"/>
       <c r="M39" s="24"/>
       <c r="N39" s="13"/>
       <c r="O39" s="77"/>
@@ -9235,8 +9248,8 @@
   </sheetPr>
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9343,11 +9356,11 @@
       <c r="A4" s="96"/>
       <c r="B4" s="96"/>
       <c r="C4" s="96"/>
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="124" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
       <c r="G4" s="96"/>
       <c r="H4" s="96"/>
       <c r="I4" s="96"/>
@@ -9693,104 +9706,104 @@
       <c r="Y14" s="96"/>
     </row>
     <row r="15" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="124"/>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="118"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="118"/>
-      <c r="M15" s="118"/>
-      <c r="N15" s="118"/>
-      <c r="O15" s="118"/>
-      <c r="P15" s="118"/>
-      <c r="Q15" s="118"/>
-      <c r="R15" s="118"/>
-      <c r="S15" s="118"/>
-      <c r="T15" s="118"/>
-      <c r="U15" s="118"/>
-      <c r="V15" s="118"/>
-      <c r="W15" s="118"/>
-      <c r="X15" s="118"/>
-      <c r="Y15" s="118"/>
+      <c r="A15" s="125"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="119"/>
+      <c r="L15" s="119"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="119"/>
+      <c r="P15" s="119"/>
+      <c r="Q15" s="119"/>
+      <c r="R15" s="119"/>
+      <c r="S15" s="119"/>
+      <c r="T15" s="119"/>
+      <c r="U15" s="119"/>
+      <c r="V15" s="119"/>
+      <c r="W15" s="119"/>
+      <c r="X15" s="119"/>
+      <c r="Y15" s="119"/>
     </row>
     <row r="16" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="118"/>
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="118"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="118"/>
-      <c r="P16" s="118"/>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="118"/>
-      <c r="S16" s="118"/>
-      <c r="T16" s="118"/>
-      <c r="U16" s="118"/>
-      <c r="V16" s="118"/>
-      <c r="W16" s="118"/>
-      <c r="X16" s="118"/>
-      <c r="Y16" s="118"/>
+      <c r="A16" s="119"/>
+      <c r="B16" s="119"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="119"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="119"/>
+      <c r="H16" s="119"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
+      <c r="M16" s="119"/>
+      <c r="N16" s="119"/>
+      <c r="O16" s="119"/>
+      <c r="P16" s="119"/>
+      <c r="Q16" s="119"/>
+      <c r="R16" s="119"/>
+      <c r="S16" s="119"/>
+      <c r="T16" s="119"/>
+      <c r="U16" s="119"/>
+      <c r="V16" s="119"/>
+      <c r="W16" s="119"/>
+      <c r="X16" s="119"/>
+      <c r="Y16" s="119"/>
     </row>
     <row r="17" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="118"/>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="118"/>
-      <c r="K17" s="118"/>
-      <c r="L17" s="118"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118"/>
-      <c r="O17" s="118"/>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="118"/>
-      <c r="S17" s="118"/>
-      <c r="T17" s="118"/>
-      <c r="U17" s="118"/>
-      <c r="V17" s="118"/>
-      <c r="W17" s="118"/>
-      <c r="X17" s="118"/>
-      <c r="Y17" s="118"/>
+      <c r="A17" s="119"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
+      <c r="M17" s="119"/>
+      <c r="N17" s="119"/>
+      <c r="O17" s="119"/>
+      <c r="P17" s="119"/>
+      <c r="Q17" s="119"/>
+      <c r="R17" s="119"/>
+      <c r="S17" s="119"/>
+      <c r="T17" s="119"/>
+      <c r="U17" s="119"/>
+      <c r="V17" s="119"/>
+      <c r="W17" s="119"/>
+      <c r="X17" s="119"/>
+      <c r="Y17" s="119"/>
     </row>
     <row r="18" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23"/>
       <c r="B18" s="24"/>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="122"/>
-      <c r="E18" s="122"/>
-      <c r="F18" s="122"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
       <c r="G18" s="24"/>
       <c r="H18" s="23"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="125" t="s">
+      <c r="J18" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="122"/>
-      <c r="L18" s="122"/>
-      <c r="M18" s="122"/>
+      <c r="K18" s="123"/>
+      <c r="L18" s="123"/>
+      <c r="M18" s="123"/>
       <c r="N18" s="13"/>
       <c r="O18" s="96"/>
       <c r="P18" s="96"/>
@@ -9882,7 +9895,7 @@
       <c r="A21" s="23"/>
       <c r="B21" s="24"/>
       <c r="C21" s="89" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D21" s="90">
         <v>2</v>
@@ -9919,7 +9932,7 @@
       <c r="A22" s="23"/>
       <c r="B22" s="24"/>
       <c r="C22" s="89" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D22" s="90">
         <v>2</v>
@@ -9954,7 +9967,7 @@
       <c r="A23" s="23"/>
       <c r="B23" s="24"/>
       <c r="C23" s="89" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D23" s="90">
         <v>1</v>
@@ -9989,7 +10002,7 @@
       <c r="A24" s="23"/>
       <c r="B24" s="24"/>
       <c r="C24" s="111" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D24" s="112">
         <v>2</v>
@@ -10024,7 +10037,7 @@
       <c r="A25" s="23"/>
       <c r="B25" s="24"/>
       <c r="C25" s="89" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D25" s="90">
         <v>1</v>
@@ -10059,7 +10072,7 @@
       <c r="A26" s="23"/>
       <c r="B26" s="24"/>
       <c r="C26" s="89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D26" s="90">
         <v>2</v>
@@ -10094,7 +10107,7 @@
       <c r="A27" s="23"/>
       <c r="B27" s="24"/>
       <c r="C27" s="89" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D27" s="90">
         <v>2</v>
@@ -10301,15 +10314,15 @@
       <c r="A34" s="23"/>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="122"/>
+      <c r="D34" s="122"/>
+      <c r="E34" s="123"/>
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
       <c r="H34" s="23"/>
       <c r="I34" s="24"/>
       <c r="J34" s="24"/>
-      <c r="K34" s="121"/>
-      <c r="L34" s="122"/>
+      <c r="K34" s="122"/>
+      <c r="L34" s="123"/>
       <c r="M34" s="24"/>
       <c r="N34" s="13"/>
       <c r="O34" s="96"/>
@@ -11882,10 +11895,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y96"/>
+  <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11992,11 +12005,11 @@
       <c r="A4" s="106"/>
       <c r="B4" s="106"/>
       <c r="C4" s="106"/>
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="124" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
       <c r="G4" s="106"/>
       <c r="H4" s="106"/>
       <c r="I4" s="106"/>
@@ -12056,7 +12069,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F6" s="19">
         <v>0</v>
@@ -12089,7 +12102,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F7" s="19">
         <v>0</v>
@@ -12122,7 +12135,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F8" s="19">
         <v>0</v>
@@ -12155,7 +12168,7 @@
         <v>17</v>
       </c>
       <c r="E9" s="19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F9" s="19">
         <v>0</v>
@@ -12188,7 +12201,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F10" s="19">
         <v>0</v>
@@ -12288,7 +12301,7 @@
       </c>
       <c r="E13" s="19">
         <f t="shared" ref="E13:F13" si="0">SUM(E6:E12)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F13" s="19">
         <f t="shared" si="0"/>
@@ -12342,104 +12355,104 @@
       <c r="Y14" s="106"/>
     </row>
     <row r="15" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="124"/>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="118"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="118"/>
-      <c r="M15" s="118"/>
-      <c r="N15" s="118"/>
-      <c r="O15" s="118"/>
-      <c r="P15" s="118"/>
-      <c r="Q15" s="118"/>
-      <c r="R15" s="118"/>
-      <c r="S15" s="118"/>
-      <c r="T15" s="118"/>
-      <c r="U15" s="118"/>
-      <c r="V15" s="118"/>
-      <c r="W15" s="118"/>
-      <c r="X15" s="118"/>
-      <c r="Y15" s="118"/>
+      <c r="A15" s="125"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="119"/>
+      <c r="L15" s="119"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="119"/>
+      <c r="P15" s="119"/>
+      <c r="Q15" s="119"/>
+      <c r="R15" s="119"/>
+      <c r="S15" s="119"/>
+      <c r="T15" s="119"/>
+      <c r="U15" s="119"/>
+      <c r="V15" s="119"/>
+      <c r="W15" s="119"/>
+      <c r="X15" s="119"/>
+      <c r="Y15" s="119"/>
     </row>
     <row r="16" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="118"/>
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="118"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="118"/>
-      <c r="P16" s="118"/>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="118"/>
-      <c r="S16" s="118"/>
-      <c r="T16" s="118"/>
-      <c r="U16" s="118"/>
-      <c r="V16" s="118"/>
-      <c r="W16" s="118"/>
-      <c r="X16" s="118"/>
-      <c r="Y16" s="118"/>
+      <c r="A16" s="119"/>
+      <c r="B16" s="119"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="119"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="119"/>
+      <c r="H16" s="119"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
+      <c r="M16" s="119"/>
+      <c r="N16" s="119"/>
+      <c r="O16" s="119"/>
+      <c r="P16" s="119"/>
+      <c r="Q16" s="119"/>
+      <c r="R16" s="119"/>
+      <c r="S16" s="119"/>
+      <c r="T16" s="119"/>
+      <c r="U16" s="119"/>
+      <c r="V16" s="119"/>
+      <c r="W16" s="119"/>
+      <c r="X16" s="119"/>
+      <c r="Y16" s="119"/>
     </row>
     <row r="17" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="118"/>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="118"/>
-      <c r="K17" s="118"/>
-      <c r="L17" s="118"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118"/>
-      <c r="O17" s="118"/>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="118"/>
-      <c r="S17" s="118"/>
-      <c r="T17" s="118"/>
-      <c r="U17" s="118"/>
-      <c r="V17" s="118"/>
-      <c r="W17" s="118"/>
-      <c r="X17" s="118"/>
-      <c r="Y17" s="118"/>
+      <c r="A17" s="119"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
+      <c r="M17" s="119"/>
+      <c r="N17" s="119"/>
+      <c r="O17" s="119"/>
+      <c r="P17" s="119"/>
+      <c r="Q17" s="119"/>
+      <c r="R17" s="119"/>
+      <c r="S17" s="119"/>
+      <c r="T17" s="119"/>
+      <c r="U17" s="119"/>
+      <c r="V17" s="119"/>
+      <c r="W17" s="119"/>
+      <c r="X17" s="119"/>
+      <c r="Y17" s="119"/>
     </row>
     <row r="18" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23"/>
       <c r="B18" s="24"/>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="122"/>
-      <c r="E18" s="122"/>
-      <c r="F18" s="122"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
       <c r="G18" s="24"/>
       <c r="H18" s="23"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="125" t="s">
+      <c r="J18" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="122"/>
-      <c r="L18" s="122"/>
-      <c r="M18" s="122"/>
+      <c r="K18" s="123"/>
+      <c r="L18" s="123"/>
+      <c r="M18" s="123"/>
       <c r="N18" s="13"/>
       <c r="O18" s="106"/>
       <c r="P18" s="106"/>
@@ -12501,10 +12514,18 @@
     <row r="20" spans="1:25" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23"/>
       <c r="B20" s="24"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="46"/>
+      <c r="C20" s="130" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20" s="90">
+        <v>1</v>
+      </c>
+      <c r="E20" s="90">
+        <v>1</v>
+      </c>
+      <c r="F20" s="91">
+        <v>2</v>
+      </c>
       <c r="G20" s="24"/>
       <c r="H20" s="23"/>
       <c r="I20" s="24"/>
@@ -12527,13 +12548,21 @@
       <c r="X20" s="106"/>
       <c r="Y20" s="106"/>
     </row>
-    <row r="21" spans="1:25" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="23"/>
       <c r="B21" s="24"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="46"/>
+      <c r="C21" s="114" t="s">
+        <v>203</v>
+      </c>
+      <c r="D21" s="44">
+        <v>1</v>
+      </c>
+      <c r="E21" s="44">
+        <v>3</v>
+      </c>
+      <c r="F21" s="46">
+        <v>4</v>
+      </c>
       <c r="G21" s="24"/>
       <c r="H21" s="23"/>
       <c r="I21" s="24"/>
@@ -12556,17 +12585,25 @@
       <c r="X21" s="106"/>
       <c r="Y21" s="106"/>
     </row>
-    <row r="22" spans="1:25" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="23"/>
       <c r="B22" s="24"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="46"/>
+      <c r="C22" s="114" t="s">
+        <v>204</v>
+      </c>
+      <c r="D22" s="44">
+        <v>2</v>
+      </c>
+      <c r="E22" s="44">
+        <v>3</v>
+      </c>
+      <c r="F22" s="46">
+        <v>4</v>
+      </c>
       <c r="G22" s="24"/>
       <c r="H22" s="23"/>
       <c r="I22" s="24"/>
-      <c r="J22" s="46"/>
+      <c r="J22" s="23"/>
       <c r="K22" s="44"/>
       <c r="L22" s="44"/>
       <c r="M22" s="46"/>
@@ -12583,7 +12620,7 @@
       <c r="X22" s="106"/>
       <c r="Y22" s="106"/>
     </row>
-    <row r="23" spans="1:25" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="23"/>
       <c r="B23" s="24"/>
       <c r="C23" s="46"/>
@@ -12610,20 +12647,20 @@
       <c r="X23" s="106"/>
       <c r="Y23" s="106"/>
     </row>
-    <row r="24" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="23"/>
       <c r="B24" s="24"/>
-      <c r="C24" s="46"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="44"/>
       <c r="E24" s="44"/>
-      <c r="F24" s="46"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="24"/>
       <c r="H24" s="23"/>
       <c r="I24" s="24"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="48"/>
       <c r="N24" s="13"/>
       <c r="O24" s="106"/>
       <c r="P24" s="106"/>
@@ -12643,11 +12680,11 @@
       <c r="C25" s="46"/>
       <c r="D25" s="44"/>
       <c r="E25" s="44"/>
-      <c r="F25" s="46"/>
+      <c r="F25" s="45"/>
       <c r="G25" s="24"/>
       <c r="H25" s="23"/>
       <c r="I25" s="24"/>
-      <c r="J25" s="46"/>
+      <c r="J25" s="43"/>
       <c r="K25" s="44"/>
       <c r="L25" s="44"/>
       <c r="M25" s="46"/>
@@ -12664,7 +12701,7 @@
       <c r="X25" s="106"/>
       <c r="Y25" s="106"/>
     </row>
-    <row r="26" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="23"/>
       <c r="B26" s="24"/>
       <c r="C26" s="46"/>
@@ -12674,10 +12711,10 @@
       <c r="G26" s="24"/>
       <c r="H26" s="23"/>
       <c r="I26" s="24"/>
-      <c r="J26" s="43"/>
+      <c r="J26" s="46"/>
       <c r="K26" s="44"/>
       <c r="L26" s="44"/>
-      <c r="M26" s="45"/>
+      <c r="M26" s="46"/>
       <c r="N26" s="13"/>
       <c r="O26" s="106"/>
       <c r="P26" s="106"/>
@@ -12691,7 +12728,7 @@
       <c r="X26" s="106"/>
       <c r="Y26" s="106"/>
     </row>
-    <row r="27" spans="1:25" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="23"/>
       <c r="B27" s="24"/>
       <c r="C27" s="46"/>
@@ -12718,10 +12755,10 @@
       <c r="X27" s="106"/>
       <c r="Y27" s="106"/>
     </row>
-    <row r="28" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="23"/>
       <c r="B28" s="24"/>
-      <c r="C28" s="43"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="44"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
@@ -12729,9 +12766,9 @@
       <c r="H28" s="23"/>
       <c r="I28" s="24"/>
       <c r="J28" s="46"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="48"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="46"/>
       <c r="N28" s="13"/>
       <c r="O28" s="106"/>
       <c r="P28" s="106"/>
@@ -12756,9 +12793,9 @@
       <c r="H29" s="23"/>
       <c r="I29" s="24"/>
       <c r="J29" s="46"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="48"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="46"/>
       <c r="N29" s="13"/>
       <c r="O29" s="106"/>
       <c r="P29" s="106"/>
@@ -12772,20 +12809,20 @@
       <c r="X29" s="106"/>
       <c r="Y29" s="106"/>
     </row>
-    <row r="30" spans="1:25" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="23"/>
       <c r="B30" s="24"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="45"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28"/>
       <c r="G30" s="24"/>
       <c r="H30" s="23"/>
       <c r="I30" s="24"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="46"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
       <c r="N30" s="13"/>
       <c r="O30" s="106"/>
       <c r="P30" s="106"/>
@@ -12799,20 +12836,30 @@
       <c r="X30" s="106"/>
       <c r="Y30" s="106"/>
     </row>
-    <row r="31" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="23"/>
       <c r="B31" s="24"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="45"/>
+      <c r="C31" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="26"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25">
+        <f>SUM(F20:F30)</f>
+        <v>10</v>
+      </c>
       <c r="G31" s="24"/>
       <c r="H31" s="23"/>
       <c r="I31" s="24"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="46"/>
+      <c r="J31" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="26"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25">
+        <f>SUM(M20:M30)</f>
+        <v>0</v>
+      </c>
       <c r="N31" s="13"/>
       <c r="O31" s="106"/>
       <c r="P31" s="106"/>
@@ -12826,20 +12873,20 @@
       <c r="X31" s="106"/>
       <c r="Y31" s="106"/>
     </row>
-    <row r="32" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="23"/>
       <c r="B32" s="24"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="45"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="122"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="24"/>
       <c r="G32" s="24"/>
       <c r="H32" s="23"/>
       <c r="I32" s="24"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="44"/>
-      <c r="M32" s="46"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="122"/>
+      <c r="L32" s="123"/>
+      <c r="M32" s="24"/>
       <c r="N32" s="13"/>
       <c r="O32" s="106"/>
       <c r="P32" s="106"/>
@@ -12853,21 +12900,21 @@
       <c r="X32" s="106"/>
       <c r="Y32" s="106"/>
     </row>
-    <row r="33" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="13"/>
+    <row r="33" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="106"/>
+      <c r="B33" s="106"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="106"/>
+      <c r="I33" s="106"/>
+      <c r="J33" s="106"/>
+      <c r="K33" s="106"/>
+      <c r="L33" s="106"/>
+      <c r="M33" s="106"/>
+      <c r="N33" s="106"/>
       <c r="O33" s="106"/>
       <c r="P33" s="106"/>
       <c r="Q33" s="106"/>
@@ -12880,21 +12927,21 @@
       <c r="X33" s="106"/>
       <c r="Y33" s="106"/>
     </row>
-    <row r="34" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="44"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="46"/>
-      <c r="N34" s="13"/>
+    <row r="34" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="106"/>
+      <c r="B34" s="106"/>
+      <c r="C34" s="106"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="106"/>
+      <c r="F34" s="106"/>
+      <c r="G34" s="106"/>
+      <c r="H34" s="106"/>
+      <c r="I34" s="106"/>
+      <c r="J34" s="106"/>
+      <c r="K34" s="106"/>
+      <c r="L34" s="106"/>
+      <c r="M34" s="106"/>
+      <c r="N34" s="106"/>
       <c r="O34" s="106"/>
       <c r="P34" s="106"/>
       <c r="Q34" s="106"/>
@@ -12907,21 +12954,21 @@
       <c r="X34" s="106"/>
       <c r="Y34" s="106"/>
     </row>
-    <row r="35" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="46"/>
-      <c r="N35" s="13"/>
+    <row r="35" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="106"/>
+      <c r="B35" s="106"/>
+      <c r="C35" s="106"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="106"/>
+      <c r="F35" s="106"/>
+      <c r="G35" s="106"/>
+      <c r="H35" s="106"/>
+      <c r="I35" s="106"/>
+      <c r="J35" s="106"/>
+      <c r="K35" s="106"/>
+      <c r="L35" s="106"/>
+      <c r="M35" s="106"/>
+      <c r="N35" s="106"/>
       <c r="O35" s="106"/>
       <c r="P35" s="106"/>
       <c r="Q35" s="106"/>
@@ -12934,21 +12981,21 @@
       <c r="X35" s="106"/>
       <c r="Y35" s="106"/>
     </row>
-    <row r="36" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="46"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="46"/>
-      <c r="N36" s="13"/>
+    <row r="36" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="106"/>
+      <c r="B36" s="106"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="106"/>
+      <c r="E36" s="106"/>
+      <c r="F36" s="106"/>
+      <c r="G36" s="106"/>
+      <c r="H36" s="106"/>
+      <c r="I36" s="106"/>
+      <c r="J36" s="106"/>
+      <c r="K36" s="106"/>
+      <c r="L36" s="106"/>
+      <c r="M36" s="106"/>
+      <c r="N36" s="106"/>
       <c r="O36" s="106"/>
       <c r="P36" s="106"/>
       <c r="Q36" s="106"/>
@@ -12961,21 +13008,21 @@
       <c r="X36" s="106"/>
       <c r="Y36" s="106"/>
     </row>
-    <row r="37" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23"/>
-      <c r="N37" s="13"/>
+    <row r="37" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="106"/>
+      <c r="B37" s="106"/>
+      <c r="C37" s="106"/>
+      <c r="D37" s="106"/>
+      <c r="E37" s="106"/>
+      <c r="F37" s="106"/>
+      <c r="G37" s="106"/>
+      <c r="H37" s="106"/>
+      <c r="I37" s="106"/>
+      <c r="J37" s="106"/>
+      <c r="K37" s="106"/>
+      <c r="L37" s="106"/>
+      <c r="M37" s="106"/>
+      <c r="N37" s="106"/>
       <c r="O37" s="106"/>
       <c r="P37" s="106"/>
       <c r="Q37" s="106"/>
@@ -12989,30 +13036,20 @@
       <c r="Y37" s="106"/>
     </row>
     <row r="38" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="26"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25">
-        <f>SUM(F20:F37)</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="24"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="K38" s="26"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25">
-        <f>SUM(M20:M37)</f>
-        <v>0</v>
-      </c>
-      <c r="N38" s="13"/>
+      <c r="A38" s="106"/>
+      <c r="B38" s="106"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="106"/>
+      <c r="G38" s="106"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="106"/>
+      <c r="K38" s="106"/>
+      <c r="L38" s="106"/>
+      <c r="M38" s="106"/>
+      <c r="N38" s="106"/>
       <c r="O38" s="106"/>
       <c r="P38" s="106"/>
       <c r="Q38" s="106"/>
@@ -13026,20 +13063,20 @@
       <c r="Y38" s="106"/>
     </row>
     <row r="39" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="121"/>
-      <c r="E39" s="122"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="121"/>
-      <c r="L39" s="122"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="13"/>
+      <c r="A39" s="106"/>
+      <c r="B39" s="106"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="106"/>
+      <c r="E39" s="106"/>
+      <c r="F39" s="106"/>
+      <c r="G39" s="106"/>
+      <c r="H39" s="106"/>
+      <c r="I39" s="106"/>
+      <c r="J39" s="106"/>
+      <c r="K39" s="106"/>
+      <c r="L39" s="106"/>
+      <c r="M39" s="106"/>
+      <c r="N39" s="106"/>
       <c r="O39" s="106"/>
       <c r="P39" s="106"/>
       <c r="Q39" s="106"/>
@@ -13056,7 +13093,7 @@
       <c r="A40" s="106"/>
       <c r="B40" s="106"/>
       <c r="C40" s="106"/>
-      <c r="D40" s="16"/>
+      <c r="D40" s="106"/>
       <c r="E40" s="106"/>
       <c r="F40" s="106"/>
       <c r="G40" s="106"/>
@@ -13083,7 +13120,7 @@
       <c r="A41" s="106"/>
       <c r="B41" s="106"/>
       <c r="C41" s="106"/>
-      <c r="D41" s="16"/>
+      <c r="D41" s="106"/>
       <c r="E41" s="106"/>
       <c r="F41" s="106"/>
       <c r="G41" s="106"/>
@@ -13110,7 +13147,7 @@
       <c r="A42" s="106"/>
       <c r="B42" s="106"/>
       <c r="C42" s="106"/>
-      <c r="D42" s="16"/>
+      <c r="D42" s="106"/>
       <c r="E42" s="106"/>
       <c r="F42" s="106"/>
       <c r="G42" s="106"/>
@@ -13596,7 +13633,7 @@
       <c r="A60" s="106"/>
       <c r="B60" s="106"/>
       <c r="C60" s="106"/>
-      <c r="D60" s="106"/>
+      <c r="D60" s="16"/>
       <c r="E60" s="106"/>
       <c r="F60" s="106"/>
       <c r="G60" s="106"/>
@@ -13623,7 +13660,7 @@
       <c r="A61" s="106"/>
       <c r="B61" s="106"/>
       <c r="C61" s="106"/>
-      <c r="D61" s="106"/>
+      <c r="D61" s="16"/>
       <c r="E61" s="106"/>
       <c r="F61" s="106"/>
       <c r="G61" s="106"/>
@@ -13650,7 +13687,7 @@
       <c r="A62" s="106"/>
       <c r="B62" s="106"/>
       <c r="C62" s="106"/>
-      <c r="D62" s="106"/>
+      <c r="D62" s="16"/>
       <c r="E62" s="106"/>
       <c r="F62" s="106"/>
       <c r="G62" s="106"/>
@@ -13677,7 +13714,7 @@
       <c r="A63" s="106"/>
       <c r="B63" s="106"/>
       <c r="C63" s="106"/>
-      <c r="D63" s="106"/>
+      <c r="D63" s="16"/>
       <c r="E63" s="106"/>
       <c r="F63" s="106"/>
       <c r="G63" s="106"/>
@@ -13704,7 +13741,7 @@
       <c r="A64" s="106"/>
       <c r="B64" s="106"/>
       <c r="C64" s="106"/>
-      <c r="D64" s="106"/>
+      <c r="D64" s="16"/>
       <c r="E64" s="106"/>
       <c r="F64" s="106"/>
       <c r="G64" s="106"/>
@@ -13731,7 +13768,7 @@
       <c r="A65" s="106"/>
       <c r="B65" s="106"/>
       <c r="C65" s="106"/>
-      <c r="D65" s="106"/>
+      <c r="D65" s="16"/>
       <c r="E65" s="106"/>
       <c r="F65" s="106"/>
       <c r="G65" s="106"/>
@@ -13758,7 +13795,7 @@
       <c r="A66" s="106"/>
       <c r="B66" s="106"/>
       <c r="C66" s="106"/>
-      <c r="D66" s="106"/>
+      <c r="D66" s="16"/>
       <c r="E66" s="106"/>
       <c r="F66" s="106"/>
       <c r="G66" s="106"/>
@@ -14402,203 +14439,14 @@
       <c r="X89" s="106"/>
       <c r="Y89" s="106"/>
     </row>
-    <row r="90" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="106"/>
-      <c r="B90" s="106"/>
-      <c r="C90" s="106"/>
-      <c r="D90" s="16"/>
-      <c r="E90" s="106"/>
-      <c r="F90" s="106"/>
-      <c r="G90" s="106"/>
-      <c r="H90" s="106"/>
-      <c r="I90" s="106"/>
-      <c r="J90" s="106"/>
-      <c r="K90" s="106"/>
-      <c r="L90" s="106"/>
-      <c r="M90" s="106"/>
-      <c r="N90" s="106"/>
-      <c r="O90" s="106"/>
-      <c r="P90" s="106"/>
-      <c r="Q90" s="106"/>
-      <c r="R90" s="106"/>
-      <c r="S90" s="106"/>
-      <c r="T90" s="106"/>
-      <c r="U90" s="106"/>
-      <c r="V90" s="106"/>
-      <c r="W90" s="106"/>
-      <c r="X90" s="106"/>
-      <c r="Y90" s="106"/>
-    </row>
-    <row r="91" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="106"/>
-      <c r="B91" s="106"/>
-      <c r="C91" s="106"/>
-      <c r="D91" s="16"/>
-      <c r="E91" s="106"/>
-      <c r="F91" s="106"/>
-      <c r="G91" s="106"/>
-      <c r="H91" s="106"/>
-      <c r="I91" s="106"/>
-      <c r="J91" s="106"/>
-      <c r="K91" s="106"/>
-      <c r="L91" s="106"/>
-      <c r="M91" s="106"/>
-      <c r="N91" s="106"/>
-      <c r="O91" s="106"/>
-      <c r="P91" s="106"/>
-      <c r="Q91" s="106"/>
-      <c r="R91" s="106"/>
-      <c r="S91" s="106"/>
-      <c r="T91" s="106"/>
-      <c r="U91" s="106"/>
-      <c r="V91" s="106"/>
-      <c r="W91" s="106"/>
-      <c r="X91" s="106"/>
-      <c r="Y91" s="106"/>
-    </row>
-    <row r="92" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="106"/>
-      <c r="B92" s="106"/>
-      <c r="C92" s="106"/>
-      <c r="D92" s="16"/>
-      <c r="E92" s="106"/>
-      <c r="F92" s="106"/>
-      <c r="G92" s="106"/>
-      <c r="H92" s="106"/>
-      <c r="I92" s="106"/>
-      <c r="J92" s="106"/>
-      <c r="K92" s="106"/>
-      <c r="L92" s="106"/>
-      <c r="M92" s="106"/>
-      <c r="N92" s="106"/>
-      <c r="O92" s="106"/>
-      <c r="P92" s="106"/>
-      <c r="Q92" s="106"/>
-      <c r="R92" s="106"/>
-      <c r="S92" s="106"/>
-      <c r="T92" s="106"/>
-      <c r="U92" s="106"/>
-      <c r="V92" s="106"/>
-      <c r="W92" s="106"/>
-      <c r="X92" s="106"/>
-      <c r="Y92" s="106"/>
-    </row>
-    <row r="93" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="106"/>
-      <c r="B93" s="106"/>
-      <c r="C93" s="106"/>
-      <c r="D93" s="16"/>
-      <c r="E93" s="106"/>
-      <c r="F93" s="106"/>
-      <c r="G93" s="106"/>
-      <c r="H93" s="106"/>
-      <c r="I93" s="106"/>
-      <c r="J93" s="106"/>
-      <c r="K93" s="106"/>
-      <c r="L93" s="106"/>
-      <c r="M93" s="106"/>
-      <c r="N93" s="106"/>
-      <c r="O93" s="106"/>
-      <c r="P93" s="106"/>
-      <c r="Q93" s="106"/>
-      <c r="R93" s="106"/>
-      <c r="S93" s="106"/>
-      <c r="T93" s="106"/>
-      <c r="U93" s="106"/>
-      <c r="V93" s="106"/>
-      <c r="W93" s="106"/>
-      <c r="X93" s="106"/>
-      <c r="Y93" s="106"/>
-    </row>
-    <row r="94" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="106"/>
-      <c r="B94" s="106"/>
-      <c r="C94" s="106"/>
-      <c r="D94" s="16"/>
-      <c r="E94" s="106"/>
-      <c r="F94" s="106"/>
-      <c r="G94" s="106"/>
-      <c r="H94" s="106"/>
-      <c r="I94" s="106"/>
-      <c r="J94" s="106"/>
-      <c r="K94" s="106"/>
-      <c r="L94" s="106"/>
-      <c r="M94" s="106"/>
-      <c r="N94" s="106"/>
-      <c r="O94" s="106"/>
-      <c r="P94" s="106"/>
-      <c r="Q94" s="106"/>
-      <c r="R94" s="106"/>
-      <c r="S94" s="106"/>
-      <c r="T94" s="106"/>
-      <c r="U94" s="106"/>
-      <c r="V94" s="106"/>
-      <c r="W94" s="106"/>
-      <c r="X94" s="106"/>
-      <c r="Y94" s="106"/>
-    </row>
-    <row r="95" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="106"/>
-      <c r="B95" s="106"/>
-      <c r="C95" s="106"/>
-      <c r="D95" s="16"/>
-      <c r="E95" s="106"/>
-      <c r="F95" s="106"/>
-      <c r="G95" s="106"/>
-      <c r="H95" s="106"/>
-      <c r="I95" s="106"/>
-      <c r="J95" s="106"/>
-      <c r="K95" s="106"/>
-      <c r="L95" s="106"/>
-      <c r="M95" s="106"/>
-      <c r="N95" s="106"/>
-      <c r="O95" s="106"/>
-      <c r="P95" s="106"/>
-      <c r="Q95" s="106"/>
-      <c r="R95" s="106"/>
-      <c r="S95" s="106"/>
-      <c r="T95" s="106"/>
-      <c r="U95" s="106"/>
-      <c r="V95" s="106"/>
-      <c r="W95" s="106"/>
-      <c r="X95" s="106"/>
-      <c r="Y95" s="106"/>
-    </row>
-    <row r="96" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="106"/>
-      <c r="B96" s="106"/>
-      <c r="C96" s="106"/>
-      <c r="D96" s="16"/>
-      <c r="E96" s="106"/>
-      <c r="F96" s="106"/>
-      <c r="G96" s="106"/>
-      <c r="H96" s="106"/>
-      <c r="I96" s="106"/>
-      <c r="J96" s="106"/>
-      <c r="K96" s="106"/>
-      <c r="L96" s="106"/>
-      <c r="M96" s="106"/>
-      <c r="N96" s="106"/>
-      <c r="O96" s="106"/>
-      <c r="P96" s="106"/>
-      <c r="Q96" s="106"/>
-      <c r="R96" s="106"/>
-      <c r="S96" s="106"/>
-      <c r="T96" s="106"/>
-      <c r="U96" s="106"/>
-      <c r="V96" s="106"/>
-      <c r="W96" s="106"/>
-      <c r="X96" s="106"/>
-      <c r="Y96" s="106"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="A15:Y17"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="J18:M18"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="K32:L32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14804,7 +14652,7 @@
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="88" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" s="33"/>
       <c r="G14" s="33"/>
@@ -14894,7 +14742,7 @@
       <c r="B21" s="33"/>
       <c r="C21" s="33"/>
       <c r="D21" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E21" s="33"/>
       <c r="F21" s="35" t="s">
@@ -15135,7 +14983,7 @@
         <v>136</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J9" s="86"/>
       <c r="K9" s="86"/>
@@ -15305,10 +15153,10 @@
     </row>
     <row r="10" spans="1:13" s="84" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="63" t="s">
         <v>156</v>
-      </c>
-      <c r="B10" s="63" t="s">
-        <v>157</v>
       </c>
       <c r="C10" s="64" t="s">
         <v>91</v>
@@ -15331,10 +15179,10 @@
     </row>
     <row r="12" spans="1:13" s="110" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="70" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C12" s="64" t="s">
         <v>91</v>
@@ -15344,13 +15192,13 @@
     </row>
     <row r="13" spans="1:13" s="110" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="70" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="64" t="s">
         <v>187</v>
-      </c>
-      <c r="B13" s="63" t="s">
-        <v>188</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>189</v>
       </c>
       <c r="D13" s="63"/>
       <c r="E13" s="63"/>
@@ -15373,7 +15221,7 @@
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="70" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B16" s="63" t="s">
         <v>97</v>
@@ -15476,10 +15324,10 @@
     </row>
     <row r="25" spans="1:5" s="109" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="70" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C25" s="64" t="s">
         <v>108</v>
@@ -15489,10 +15337,10 @@
     </row>
     <row r="26" spans="1:5" s="109" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="70" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B26" s="63" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C26" s="64" t="s">
         <v>108</v>
@@ -15588,10 +15436,10 @@
     </row>
     <row r="35" spans="1:5" s="110" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A35" s="70" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B35" s="63" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C35" s="64"/>
       <c r="D35" s="63"/>
@@ -15599,10 +15447,10 @@
     </row>
     <row r="36" spans="1:5" s="110" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A36" s="70" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B36" s="63" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C36" s="64"/>
       <c r="D36" s="63"/>
@@ -15626,7 +15474,7 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="108" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B39" s="63" t="s">
         <v>126</v>
@@ -15639,7 +15487,7 @@
     </row>
     <row r="40" spans="1:5" s="104" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="108" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B40" s="63" t="s">
         <v>126</v>
@@ -15652,7 +15500,7 @@
     </row>
     <row r="41" spans="1:5" s="104" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="108" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B41" s="63" t="s">
         <v>126</v>
@@ -15678,7 +15526,7 @@
     </row>
     <row r="43" spans="1:5" s="56" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="70" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B43" s="63" t="s">
         <v>127</v>
@@ -15691,7 +15539,7 @@
     </row>
     <row r="44" spans="1:5" s="56" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B44" s="63" t="s">
         <v>127</v>
@@ -15704,10 +15552,10 @@
     </row>
     <row r="45" spans="1:5" s="104" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="108" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B45" s="63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C45" s="64" t="s">
         <v>128</v>
@@ -15717,10 +15565,10 @@
     </row>
     <row r="46" spans="1:5" s="104" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="108" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B46" s="63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C46" s="64" t="s">
         <v>128</v>
@@ -15730,10 +15578,10 @@
     </row>
     <row r="47" spans="1:5" s="104" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="108" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B47" s="63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C47" s="64" t="s">
         <v>128</v>
@@ -15743,10 +15591,10 @@
     </row>
     <row r="48" spans="1:5" s="93" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B48" s="94" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C48" s="64" t="s">
         <v>128</v>
@@ -15756,10 +15604,10 @@
     </row>
     <row r="49" spans="1:5" s="93" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B49" s="94" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C49" s="64" t="s">
         <v>128</v>
@@ -15769,10 +15617,10 @@
     </row>
     <row r="50" spans="1:5" s="93" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A50" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" s="94" t="s">
         <v>165</v>
-      </c>
-      <c r="B50" s="94" t="s">
-        <v>166</v>
       </c>
       <c r="C50" s="64" t="s">
         <v>128</v>
@@ -15798,7 +15646,7 @@
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="70" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B53" s="63" t="s">
         <v>130</v>

</xml_diff>